<commit_message>
Added new API testing keyword actions to the snj-selenium-java-keywords document available under src/main/resources -> keywords folder.
</commit_message>
<xml_diff>
--- a/src/main/resources/keywords/snj-selenium-java-keywords.xlsx
+++ b/src/main/resources/keywords/snj-selenium-java-keywords.xlsx
@@ -12,19 +12,21 @@
     <sheet name="UtilityActions" sheetId="2" r:id="rId3"/>
     <sheet name="ValidationActions" sheetId="4" r:id="rId4"/>
     <sheet name="WebActions" sheetId="5" r:id="rId5"/>
-    <sheet name="AutomationEngine" sheetId="6" r:id="rId6"/>
-    <sheet name="CSVDataHandler" sheetId="7" r:id="rId7"/>
-    <sheet name="ExcelDataHandler" sheetId="8" r:id="rId8"/>
-    <sheet name="PropertyDataHandler" sheetId="9" r:id="rId9"/>
-    <sheet name="DatabaseActions" sheetId="10" r:id="rId10"/>
-    <sheet name="AutomationReport" sheetId="1" r:id="rId11"/>
+    <sheet name="DatabaseActions" sheetId="10" r:id="rId6"/>
+    <sheet name="APIActions" sheetId="12" r:id="rId7"/>
+    <sheet name="APIValidationActions" sheetId="13" r:id="rId8"/>
+    <sheet name="ExcelDataHandler" sheetId="8" r:id="rId9"/>
+    <sheet name="CSVDataHandler" sheetId="7" r:id="rId10"/>
+    <sheet name="PropertyDataHandler" sheetId="9" r:id="rId11"/>
+    <sheet name="AutomationEngine" sheetId="6" r:id="rId12"/>
+    <sheet name="AutomationReport" sheetId="1" r:id="rId13"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="340">
   <si>
     <t>Keywords</t>
   </si>
@@ -888,6 +890,162 @@
   </si>
   <si>
     <t xml:space="preserve">verifyElementEnabled(org.openqa.selenium.WebDriver,java.lang.String,java.lang.String,java.lang.String,java.lang.String) </t>
+  </si>
+  <si>
+    <t>APIActions</t>
+  </si>
+  <si>
+    <t>getRequest(java.lang.String,java.lang.String)</t>
+  </si>
+  <si>
+    <t>Perform simple HTTP Get request</t>
+  </si>
+  <si>
+    <t>Perform simple HTTP Delete request</t>
+  </si>
+  <si>
+    <t>getRequestWithAuthToken(java.lang.String,java.lang.String,java.lang.String,java.lang.String,java.lang.String)</t>
+  </si>
+  <si>
+    <t>Perform HTTP Get request with authorization token</t>
+  </si>
+  <si>
+    <t>Perform HTTP Get request with multiple query parameters</t>
+  </si>
+  <si>
+    <t>getRequestWithMultipleQueries(java.lang.String,java.util.Map&lt;String, String&gt;,java.lang.String)</t>
+  </si>
+  <si>
+    <t>Perform HTTP Get request with path parameter</t>
+  </si>
+  <si>
+    <t>Perform HTTP Get request with query parameter</t>
+  </si>
+  <si>
+    <t>Perform HTTP Delete request with multiple path parameters</t>
+  </si>
+  <si>
+    <t>getRequestWithPathParameter(java.lang.String,java.lang.String,java.lang.String,java.lang.String)</t>
+  </si>
+  <si>
+    <t>getRequestWithQueryParameter(java.lang.String,java.lang.String,java.lang.String,java.lang.String)</t>
+  </si>
+  <si>
+    <t>Perform HTTP Post request with body data from file</t>
+  </si>
+  <si>
+    <t>Perform HTTP Post request with in-line body data</t>
+  </si>
+  <si>
+    <t>Perform HTTP Put request with in-line body data</t>
+  </si>
+  <si>
+    <t>postRequest(java.lang.String,java.lang.String,java.util.Map&lt;String, String&gt;,java.util.Map&lt;String, String&gt;,java.lang.String)</t>
+  </si>
+  <si>
+    <t>Perform simple HTTP Put request with body data from file</t>
+  </si>
+  <si>
+    <t>postRequest(java.lang.String,java.lang.String,java.lang.String,java.lang.String)</t>
+  </si>
+  <si>
+    <t>putRequest(java.lang.String,java.lang.String,java.lang.String,java.lang.String)</t>
+  </si>
+  <si>
+    <t>putRequest(java.lang.String,java.lang.String,java.lang.String,java.lang.String,java.lang.String,java.lang.String)</t>
+  </si>
+  <si>
+    <t>Perform HTTP Put request with body data from file and using path parameter and path value</t>
+  </si>
+  <si>
+    <t>putRequest(java.lang.String,java.util.Map&lt;String, String&gt;,java.util.Map&lt;String, String&gt;,java.lang.String,java.lang.String)</t>
+  </si>
+  <si>
+    <t>deleteRequest(java.lang.String,java.lang.String)</t>
+  </si>
+  <si>
+    <t>Perform HTTP Delete request with a given path parameter</t>
+  </si>
+  <si>
+    <t>deleteRequestWithPathParameter(java.lang.String,java.lang.String,java.lang.String,java.lang.String)</t>
+  </si>
+  <si>
+    <t>deleteRequestWithMultiplePathParameters(java.lang.String,java.util.Map&lt;String, String&gt;,java.lang.String)</t>
+  </si>
+  <si>
+    <t>APIValidationActions</t>
+  </si>
+  <si>
+    <t>Get the value from JSON response</t>
+  </si>
+  <si>
+    <t>printAllHeaders(io.restassured.response.Response)</t>
+  </si>
+  <si>
+    <t>Print all header names and values</t>
+  </si>
+  <si>
+    <t>Validate the ContentType from the response</t>
+  </si>
+  <si>
+    <t>Validate the SessionId from the response</t>
+  </si>
+  <si>
+    <t>Validate the header from the response</t>
+  </si>
+  <si>
+    <t>validateHeader(io.restassured.response.Response,java.lang.String, java.lang.String)</t>
+  </si>
+  <si>
+    <t>validateContentType(io.restassured.response.Response, java.lang.String)</t>
+  </si>
+  <si>
+    <t>getValueFromResponse(io.restassured.response.Response,java.lang.String)</t>
+  </si>
+  <si>
+    <t>validateJsonPath(io.restassured.response.Response,java.lang.String)</t>
+  </si>
+  <si>
+    <t>Validate JsonPath from the response</t>
+  </si>
+  <si>
+    <t>validateJsonPathToBooleanValue(io.restassured.response.Response,java.lang.String,boolean)</t>
+  </si>
+  <si>
+    <t>Validate JsonPath to boolean value</t>
+  </si>
+  <si>
+    <t>Validate JsonPath to integer value</t>
+  </si>
+  <si>
+    <t>validateJsonPathToIntegerValue(io.restassured.response.Response,java.lang.String,int)</t>
+  </si>
+  <si>
+    <t>Validate JsonPath to null value</t>
+  </si>
+  <si>
+    <t>Validate JsonPath to string value</t>
+  </si>
+  <si>
+    <t>validateJsonPathToNullValue(io.restassured.response.Response,java.lang.String)</t>
+  </si>
+  <si>
+    <t>validateJsonPathToStringValue(io.restassured.response.Response,java.lang.String,java.lang.String)</t>
+  </si>
+  <si>
+    <t>validateSessionId(io.restassured.response.Response,java.lang.String)</t>
+  </si>
+  <si>
+    <t>Validate the status code from the response</t>
+  </si>
+  <si>
+    <t>validateStatusCode(io.restassured.response.Response,int)</t>
+  </si>
+  <si>
+    <t>validateStatusLine(io.restassured.response.Response,java.lang.String)</t>
+  </si>
+  <si>
+    <t>Validate the status line from the response</t>
   </si>
 </sst>
 </file>
@@ -974,7 +1132,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -1279,12 +1437,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1385,13 +1558,28 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1474,6 +1662,128 @@
 </file>
 
 <file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Left Arrow 1">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12011025" y="19050"/>
+          <a:ext cx="409575" cy="171450"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-IN" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Left Arrow 1">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12001500" y="19050"/>
+          <a:ext cx="409575" cy="171450"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-IN" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1722,15 +2032,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
+      <xdr:colOff>95250</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
+      <xdr:colOff>504825</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1741,7 +2051,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12001500" y="19050"/>
+          <a:off x="12011025" y="9525"/>
           <a:ext cx="409575" cy="171450"/>
         </a:xfrm>
         <a:prstGeom prst="leftArrow">
@@ -1783,15 +2093,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
+      <xdr:colOff>85725</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>19051</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
+      <xdr:colOff>495300</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:rowOff>190501</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1802,7 +2112,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11982450" y="9525"/>
+          <a:off x="12001500" y="19051"/>
           <a:ext cx="409575" cy="171450"/>
         </a:xfrm>
         <a:prstGeom prst="leftArrow">
@@ -1905,15 +2215,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
+      <xdr:colOff>104775</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
+      <xdr:colOff>514350</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1924,7 +2234,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12011025" y="19050"/>
+          <a:off x="12020550" y="9525"/>
           <a:ext cx="409575" cy="171450"/>
         </a:xfrm>
         <a:prstGeom prst="leftArrow">
@@ -1966,13 +2276,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
+      <xdr:colOff>66675</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
+      <xdr:colOff>476250</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
@@ -1985,7 +2295,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12011025" y="9525"/>
+          <a:off x="11982450" y="9525"/>
           <a:ext cx="409575" cy="171450"/>
         </a:xfrm>
         <a:prstGeom prst="leftArrow">
@@ -2309,10 +2619,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:D14"/>
+  <dimension ref="C2:D16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2323,10 +2633,10 @@
   <sheetData>
     <row r="2" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="3:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="35" t="s">
         <v>174</v>
       </c>
-      <c r="D3" s="35"/>
+      <c r="D3" s="36"/>
     </row>
     <row r="4" spans="3:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="26" t="s">
@@ -2362,59 +2672,75 @@
     </row>
     <row r="8" spans="3:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="26" t="s">
-        <v>8</v>
+        <v>288</v>
       </c>
       <c r="D8" s="28">
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="3:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="26" t="s">
-        <v>9</v>
+        <v>315</v>
       </c>
       <c r="D9" s="28">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="3:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="26" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D10" s="28">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="3:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D11" s="28">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="3:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="26" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D12" s="28">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="3:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="3:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="3:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="28">
+      <c r="D15" s="28">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="27" t="s">
+    <row r="16" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="27" t="s">
         <v>175</v>
       </c>
-      <c r="D14" s="25">
-        <f>SUM(D4:D13)</f>
-        <v>138</v>
+      <c r="D16" s="25">
+        <f>SUM(D4:D15)</f>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -2426,12 +2752,14 @@
     <hyperlink ref="C5" location="UtilityActions!A1" display="UtilityActions"/>
     <hyperlink ref="C6" location="ValidationActions!A1" display="ValidationActions"/>
     <hyperlink ref="C7" location="WebActions!A1" display="WebActions"/>
-    <hyperlink ref="C8" location="AutomationEngine!A1" display="AutomationEngine"/>
-    <hyperlink ref="C9" location="CSVDataHandler!A1" display="CSVDataHandler"/>
-    <hyperlink ref="C10" location="ExcelDataHandler!A1" display="ExcelDataHandler"/>
-    <hyperlink ref="C11" location="PropertyDataHandler!A1" display="PropertyDataHandler"/>
-    <hyperlink ref="C12" location="DatabaseActions!A1" display="DatabaseActions"/>
-    <hyperlink ref="C13" location="AutomationReport!A1" display="AutomationReport"/>
+    <hyperlink ref="C10" location="AutomationEngine!A1" display="AutomationEngine"/>
+    <hyperlink ref="C11" location="CSVDataHandler!A1" display="CSVDataHandler"/>
+    <hyperlink ref="C12" location="ExcelDataHandler!A1" display="ExcelDataHandler"/>
+    <hyperlink ref="C13" location="PropertyDataHandler!A1" display="PropertyDataHandler"/>
+    <hyperlink ref="C14" location="DatabaseActions!A1" display="DatabaseActions"/>
+    <hyperlink ref="C15" location="AutomationReport!A1" display="AutomationReport"/>
+    <hyperlink ref="C8" location="APIActions!A1" display="APIActions"/>
+    <hyperlink ref="C9" location="APIValidationActions!A1" display="APIValidationActions"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2440,11 +2768,11 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2469,74 +2797,32 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="16">
         <v>1</v>
       </c>
-      <c r="B2" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="16">
+      <c r="B2" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="17">
         <v>2</v>
       </c>
-      <c r="B3" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="16">
-        <v>3</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="16">
-        <v>4</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="17">
-        <v>5</v>
-      </c>
-      <c r="B6" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="33" t="s">
-        <v>168</v>
-      </c>
-      <c r="D6" s="31" t="s">
-        <v>169</v>
+      <c r="B3" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>139</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -2547,6 +2833,124 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="3" max="3" width="93.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="56.42578125" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="17">
+        <v>1</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="D2" s="23" t="s">
+        <v>159</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="3" max="3" width="93.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="56.42578125" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="16">
+        <v>1</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="17">
+        <v>2</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>137</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>140</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -2840,7 +3244,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="36">
+      <c r="A16" s="34">
         <v>15</v>
       </c>
       <c r="B16" s="29" t="s">
@@ -4104,7 +4508,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4418,11 +4822,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4452,27 +4856,69 @@
         <v>1</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>136</v>
+        <v>167</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="17">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="16">
         <v>2</v>
       </c>
-      <c r="B3" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="33" t="s">
-        <v>137</v>
-      </c>
-      <c r="D3" s="31" t="s">
-        <v>140</v>
+      <c r="B3" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="16">
+        <v>3</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="16">
+        <v>4</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="17">
+        <v>5</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>168</v>
+      </c>
+      <c r="D6" s="31" t="s">
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -4484,11 +4930,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4513,35 +4959,192 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="16">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="19" t="s">
+        <v>288</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>289</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="15">
+        <v>2</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>288</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>292</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="16">
+        <v>3</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>288</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>295</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="15">
+        <v>4</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>288</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>299</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="16">
+        <v>5</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>288</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>300</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="15">
+        <v>6</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>288</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>306</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="16">
+        <v>7</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>288</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>304</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="15">
+        <v>8</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>288</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>307</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="16">
         <v>9</v>
       </c>
-      <c r="C2" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="17">
-        <v>2</v>
-      </c>
-      <c r="B3" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="32" t="s">
-        <v>139</v>
-      </c>
-      <c r="D3" s="23" t="s">
-        <v>143</v>
+      <c r="B10" s="19" t="s">
+        <v>288</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>308</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="15">
+        <v>10</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>288</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>310</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="16">
+        <v>11</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>288</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>311</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="15">
+        <v>12</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>288</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>314</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="16">
+        <v>13</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>288</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>313</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>312</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="C2:C14">
+    <sortCondition ref="C1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -4549,6 +5152,215 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="3" max="3" width="93.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="56.42578125" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="39" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="40">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="40">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="40">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="40">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="40">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="40">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="40">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="40">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>333</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="40">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="40">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="40">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="41">
+        <v>12</v>
+      </c>
+      <c r="B13" s="33" t="s">
+        <v>315</v>
+      </c>
+      <c r="C13" s="33" t="s">
+        <v>338</v>
+      </c>
+      <c r="D13" s="31" t="s">
+        <v>339</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="C2:C13">
+    <sortCondition ref="C1"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
@@ -4696,56 +5508,4 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
-    <col min="3" max="3" width="93.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="56.42578125" style="3" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="17">
-        <v>1</v>
-      </c>
-      <c r="B2" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>158</v>
-      </c>
-      <c r="D2" s="23" t="s">
-        <v>159</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added new keyword actions. Updated snj-selenium-java-keywords document.
</commit_message>
<xml_diff>
--- a/src/main/resources/keywords/snj-selenium-java-keywords.xlsx
+++ b/src/main/resources/keywords/snj-selenium-java-keywords.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="348">
   <si>
     <t>Keywords</t>
   </si>
@@ -1046,6 +1046,30 @@
   </si>
   <si>
     <t>Validate the status line from the response</t>
+  </si>
+  <si>
+    <t>doBasicAuthentication(org.openqa.selenium.WebDriver,java.lang.String,java.lang.String)</t>
+  </si>
+  <si>
+    <t>To do the basic authentication</t>
+  </si>
+  <si>
+    <t>simulateDeviceMode(org.openqa.selenium.WebDriver,int,int,boolean,int)</t>
+  </si>
+  <si>
+    <t>Simulate device mode and set different screen resolutions</t>
+  </si>
+  <si>
+    <t>simulateNetworkSpeed(org.openqa.selenium.WebDriver,boolean,int,int,int,java.lang.String)</t>
+  </si>
+  <si>
+    <t>Simulate network speed 2G,3G,4G,BLUETOOTH,ETHERNET,WIFI,WIMAX and also offline mode</t>
+  </si>
+  <si>
+    <t>mockGeolocation(org.openqa.selenium.WebDriver,double,double,int)</t>
+  </si>
+  <si>
+    <t>Mock geolocation based on latitude, longitude and accuracy</t>
   </si>
 </sst>
 </file>
@@ -1561,12 +1585,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1580,6 +1598,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2622,7 +2646,7 @@
   <dimension ref="C2:D16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2633,10 +2657,10 @@
   <sheetData>
     <row r="2" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="3:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="40" t="s">
         <v>174</v>
       </c>
-      <c r="D3" s="36"/>
+      <c r="D3" s="41"/>
     </row>
     <row r="4" spans="3:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="26" t="s">
@@ -2651,7 +2675,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="28">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="3:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -2740,7 +2764,7 @@
       </c>
       <c r="D16" s="25">
         <f>SUM(D4:D15)</f>
-        <v>163</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -3266,11 +3290,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3281,25 +3305,25 @@
     <col min="4" max="4" width="56.42578125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="37" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="16">
+      <c r="A2" s="38">
         <v>1</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="21" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="21" t="s">
@@ -3310,10 +3334,10 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="16">
+      <c r="A3" s="38">
         <v>2</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="21" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="21" t="s">
@@ -3324,10 +3348,10 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="16">
+      <c r="A4" s="38">
         <v>3</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="21" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="21" t="s">
@@ -3338,10 +3362,10 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="16">
+      <c r="A5" s="38">
         <v>4</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="21" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="21" t="s">
@@ -3352,10 +3376,10 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="16">
-        <v>5</v>
-      </c>
-      <c r="B6" s="18" t="s">
+      <c r="A6" s="38">
+        <v>5</v>
+      </c>
+      <c r="B6" s="21" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="21" t="s">
@@ -3366,10 +3390,10 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="16">
+      <c r="A7" s="38">
         <v>6</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="21" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="21" t="s">
@@ -3380,10 +3404,10 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="16">
+      <c r="A8" s="38">
         <v>7</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="21" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="21" t="s">
@@ -3394,10 +3418,10 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="16">
+      <c r="A9" s="38">
         <v>8</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="21" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="19" t="s">
@@ -3408,10 +3432,10 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="16">
+      <c r="A10" s="38">
         <v>9</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="21" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="19" t="s">
@@ -3422,10 +3446,10 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="16">
+      <c r="A11" s="38">
         <v>10</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="21" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="21" t="s">
@@ -3436,10 +3460,10 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="16">
+      <c r="A12" s="38">
         <v>11</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="21" t="s">
         <v>5</v>
       </c>
       <c r="C12" s="21" t="s">
@@ -3450,520 +3474,576 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="16">
+      <c r="A13" s="38">
         <v>12</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="21" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="21" t="s">
+        <v>340</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="38">
+        <v>13</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="D13" s="20" t="s">
+      <c r="D14" s="20" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="16">
-        <v>13</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="21" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="38">
+        <v>14</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="D14" s="20" t="s">
+      <c r="D15" s="20" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="16">
-        <v>14</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="21" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="38">
+        <v>15</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="D15" s="20" t="s">
+      <c r="D16" s="20" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="16">
-        <v>15</v>
-      </c>
-      <c r="B16" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="19" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="38">
+        <v>16</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="D16" s="20" t="s">
+      <c r="D17" s="20" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="16">
-        <v>16</v>
-      </c>
-      <c r="B17" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="21" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="38">
+        <v>17</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="D17" s="20" t="s">
+      <c r="D18" s="20" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="16">
-        <v>17</v>
-      </c>
-      <c r="B18" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="21" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="38">
+        <v>18</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="D18" s="20" t="s">
+      <c r="D19" s="20" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="16">
-        <v>18</v>
-      </c>
-      <c r="B19" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="19" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="38">
+        <v>19</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="D19" s="20" t="s">
+      <c r="D20" s="20" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="16">
-        <v>19</v>
-      </c>
-      <c r="B20" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="19" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="38">
+        <v>20</v>
+      </c>
+      <c r="B21" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="D20" s="20" t="s">
+      <c r="D21" s="20" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="16">
-        <v>20</v>
-      </c>
-      <c r="B21" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="21" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="38">
+        <v>21</v>
+      </c>
+      <c r="B22" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="D21" s="20" t="s">
+      <c r="D22" s="20" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="16">
-        <v>21</v>
-      </c>
-      <c r="B22" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" s="19" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="38">
+        <v>22</v>
+      </c>
+      <c r="B23" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="D22" s="20" t="s">
+      <c r="D23" s="20" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="16">
-        <v>22</v>
-      </c>
-      <c r="B23" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" s="19" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="38">
+        <v>23</v>
+      </c>
+      <c r="B24" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="D23" s="20" t="s">
+      <c r="D24" s="20" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="16">
-        <v>23</v>
-      </c>
-      <c r="B24" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" s="21" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="38">
+        <v>24</v>
+      </c>
+      <c r="B25" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="D24" s="20" t="s">
+      <c r="D25" s="20" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="16">
-        <v>24</v>
-      </c>
-      <c r="B25" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" s="19" t="s">
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="38">
+        <v>25</v>
+      </c>
+      <c r="B26" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="D25" s="20" t="s">
+      <c r="D26" s="20" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="16">
-        <v>25</v>
-      </c>
-      <c r="B26" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" s="21" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="38">
+        <v>26</v>
+      </c>
+      <c r="B27" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="D26" s="20" t="s">
+      <c r="D27" s="20" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="16">
-        <v>26</v>
-      </c>
-      <c r="B27" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" s="21" t="s">
+    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="38">
+        <v>27</v>
+      </c>
+      <c r="B28" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="D27" s="20" t="s">
+      <c r="D28" s="20" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="16">
-        <v>27</v>
-      </c>
-      <c r="B28" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" s="21" t="s">
+    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="38">
+        <v>28</v>
+      </c>
+      <c r="B29" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="D28" s="20" t="s">
+      <c r="D29" s="20" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="16">
-        <v>28</v>
-      </c>
-      <c r="B29" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C29" s="21" t="s">
+    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="38">
+        <v>29</v>
+      </c>
+      <c r="B30" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="D29" s="20" t="s">
+      <c r="D30" s="20" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="16">
-        <v>29</v>
-      </c>
-      <c r="B30" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C30" s="19" t="s">
+    <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="38">
+        <v>30</v>
+      </c>
+      <c r="B31" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" s="19" t="s">
         <v>270</v>
       </c>
-      <c r="D30" s="20" t="s">
+      <c r="D31" s="20" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="16">
-        <v>30</v>
-      </c>
-      <c r="B31" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C31" s="21" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="38">
+        <v>31</v>
+      </c>
+      <c r="B32" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" s="19" t="s">
+        <v>346</v>
+      </c>
+      <c r="D32" s="20" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="38">
+        <v>32</v>
+      </c>
+      <c r="B33" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="D31" s="20" t="s">
+      <c r="D33" s="20" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="16">
-        <v>31</v>
-      </c>
-      <c r="B32" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C32" s="21" t="s">
+    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="38">
+        <v>33</v>
+      </c>
+      <c r="B34" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="D32" s="20" t="s">
+      <c r="D34" s="20" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="16">
-        <v>32</v>
-      </c>
-      <c r="B33" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C33" s="21" t="s">
+    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="38">
+        <v>34</v>
+      </c>
+      <c r="B35" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="D33" s="20" t="s">
+      <c r="D35" s="20" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="16">
-        <v>33</v>
-      </c>
-      <c r="B34" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C34" s="21" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="38">
+        <v>35</v>
+      </c>
+      <c r="B36" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="D34" s="20" t="s">
+      <c r="D36" s="20" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="16">
-        <v>34</v>
-      </c>
-      <c r="B35" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C35" s="21" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="38">
+        <v>36</v>
+      </c>
+      <c r="B37" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="D35" s="20" t="s">
+      <c r="D37" s="20" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="16">
-        <v>35</v>
-      </c>
-      <c r="B36" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C36" s="21" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="38">
+        <v>37</v>
+      </c>
+      <c r="B38" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="D36" s="20" t="s">
+      <c r="D38" s="20" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="16">
-        <v>36</v>
-      </c>
-      <c r="B37" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C37" s="21" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="38">
+        <v>38</v>
+      </c>
+      <c r="B39" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="D37" s="20" t="s">
+      <c r="D39" s="20" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="16">
-        <v>37</v>
-      </c>
-      <c r="B38" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C38" s="21" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="38">
+        <v>39</v>
+      </c>
+      <c r="B40" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="D38" s="20" t="s">
+      <c r="D40" s="20" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="16">
-        <v>38</v>
-      </c>
-      <c r="B39" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C39" s="19" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="38">
+        <v>40</v>
+      </c>
+      <c r="B41" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="D39" s="20" t="s">
+      <c r="D41" s="20" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="16">
-        <v>39</v>
-      </c>
-      <c r="B40" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C40" s="19" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="38">
+        <v>41</v>
+      </c>
+      <c r="B42" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="D40" s="20" t="s">
+      <c r="D42" s="20" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="16">
-        <v>40</v>
-      </c>
-      <c r="B41" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C41" s="19" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="38">
+        <v>42</v>
+      </c>
+      <c r="B43" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="D41" s="20" t="s">
+      <c r="D43" s="20" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="16">
-        <v>41</v>
-      </c>
-      <c r="B42" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C42" s="19" t="s">
+    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="38">
+        <v>43</v>
+      </c>
+      <c r="B44" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="D42" s="20" t="s">
+      <c r="D44" s="20" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="16">
-        <v>42</v>
-      </c>
-      <c r="B43" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C43" s="21" t="s">
+    <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="38">
+        <v>44</v>
+      </c>
+      <c r="B45" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C45" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="D43" s="20" t="s">
+      <c r="D45" s="20" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="16">
-        <v>43</v>
-      </c>
-      <c r="B44" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C44" s="21" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="38">
+        <v>45</v>
+      </c>
+      <c r="B46" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46" s="21" t="s">
+        <v>342</v>
+      </c>
+      <c r="D46" s="20" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A47" s="38">
+        <v>46</v>
+      </c>
+      <c r="B47" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C47" s="21" t="s">
+        <v>344</v>
+      </c>
+      <c r="D47" s="20" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" s="38">
+        <v>47</v>
+      </c>
+      <c r="B48" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C48" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="D44" s="20" t="s">
+      <c r="D48" s="20" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="16">
+    <row r="49" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="38">
+        <v>48</v>
+      </c>
+      <c r="B49" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C49" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D49" s="20" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" s="38">
+        <v>49</v>
+      </c>
+      <c r="B50" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C50" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="D50" s="20" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="38">
+        <v>50</v>
+      </c>
+      <c r="B51" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C51" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="D51" s="20" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" s="38">
+        <v>51</v>
+      </c>
+      <c r="B52" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C52" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B45" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C45" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="D45" s="20" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="16">
-        <v>45</v>
-      </c>
-      <c r="B46" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C46" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="D46" s="20" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A47" s="16">
-        <v>46</v>
-      </c>
-      <c r="B47" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C47" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="D47" s="20" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A48" s="16">
-        <v>47</v>
-      </c>
-      <c r="B48" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C48" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="D48" s="20" t="s">
+      <c r="D52" s="20" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="17">
-        <v>48</v>
-      </c>
-      <c r="B49" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="C49" s="32" t="s">
+    <row r="53" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="39">
+        <v>52</v>
+      </c>
+      <c r="B53" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="D49" s="23" t="s">
+      <c r="D53" s="23" t="s">
         <v>220</v>
       </c>
     </row>
@@ -5169,21 +5249,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="37" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="40">
+      <c r="A2" s="38">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -5197,7 +5277,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="40">
+      <c r="A3" s="38">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -5211,7 +5291,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="40">
+      <c r="A4" s="38">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -5225,7 +5305,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="40">
+      <c r="A5" s="38">
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -5239,7 +5319,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="40">
+      <c r="A6" s="38">
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -5253,7 +5333,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="40">
+      <c r="A7" s="38">
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -5267,7 +5347,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="40">
+      <c r="A8" s="38">
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -5281,7 +5361,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="40">
+      <c r="A9" s="38">
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -5295,7 +5375,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="40">
+      <c r="A10" s="38">
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -5309,7 +5389,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="40">
+      <c r="A11" s="38">
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -5323,7 +5403,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="40">
+      <c r="A12" s="38">
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -5337,7 +5417,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="41">
+      <c r="A13" s="39">
         <v>12</v>
       </c>
       <c r="B13" s="33" t="s">

</xml_diff>

<commit_message>
Updated snj-selenium-java-keywords document file.
</commit_message>
<xml_diff>
--- a/src/main/resources/keywords/snj-selenium-java-keywords.xlsx
+++ b/src/main/resources/keywords/snj-selenium-java-keywords.xlsx
@@ -14,19 +14,20 @@
     <sheet name="WebActions" sheetId="5" r:id="rId5"/>
     <sheet name="DatabaseActions" sheetId="10" r:id="rId6"/>
     <sheet name="APIActions" sheetId="12" r:id="rId7"/>
-    <sheet name="APIValidationActions" sheetId="13" r:id="rId8"/>
-    <sheet name="ExcelDataHandler" sheetId="8" r:id="rId9"/>
-    <sheet name="CSVDataHandler" sheetId="7" r:id="rId10"/>
-    <sheet name="PropertyDataHandler" sheetId="9" r:id="rId11"/>
-    <sheet name="AutomationEngine" sheetId="6" r:id="rId12"/>
-    <sheet name="AutomationReport" sheetId="1" r:id="rId13"/>
+    <sheet name="APIValidations" sheetId="13" r:id="rId8"/>
+    <sheet name="APIUtilities" sheetId="14" r:id="rId9"/>
+    <sheet name="ExcelDataHandler" sheetId="8" r:id="rId10"/>
+    <sheet name="CSVDataHandler" sheetId="7" r:id="rId11"/>
+    <sheet name="PropertyDataHandler" sheetId="9" r:id="rId12"/>
+    <sheet name="AutomationEngine" sheetId="6" r:id="rId13"/>
+    <sheet name="AutomationReport" sheetId="1" r:id="rId14"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="349">
   <si>
     <t>Keywords</t>
   </si>
@@ -913,33 +914,12 @@
     <t>Perform HTTP Get request with multiple query parameters</t>
   </si>
   <si>
-    <t>getRequestWithMultipleQueries(java.lang.String,java.util.Map&lt;String, String&gt;,java.lang.String)</t>
-  </si>
-  <si>
-    <t>Perform HTTP Get request with path parameter</t>
-  </si>
-  <si>
-    <t>Perform HTTP Get request with query parameter</t>
-  </si>
-  <si>
-    <t>Perform HTTP Delete request with multiple path parameters</t>
-  </si>
-  <si>
-    <t>getRequestWithPathParameter(java.lang.String,java.lang.String,java.lang.String,java.lang.String)</t>
-  </si>
-  <si>
-    <t>getRequestWithQueryParameter(java.lang.String,java.lang.String,java.lang.String,java.lang.String)</t>
-  </si>
-  <si>
     <t>Perform HTTP Post request with body data from file</t>
   </si>
   <si>
     <t>Perform HTTP Post request with in-line body data</t>
   </si>
   <si>
-    <t>Perform HTTP Put request with in-line body data</t>
-  </si>
-  <si>
     <t>postRequest(java.lang.String,java.lang.String,java.util.Map&lt;String, String&gt;,java.util.Map&lt;String, String&gt;,java.lang.String)</t>
   </si>
   <si>
@@ -952,39 +932,18 @@
     <t>putRequest(java.lang.String,java.lang.String,java.lang.String,java.lang.String)</t>
   </si>
   <si>
-    <t>putRequest(java.lang.String,java.lang.String,java.lang.String,java.lang.String,java.lang.String,java.lang.String)</t>
-  </si>
-  <si>
-    <t>Perform HTTP Put request with body data from file and using path parameter and path value</t>
-  </si>
-  <si>
     <t>putRequest(java.lang.String,java.util.Map&lt;String, String&gt;,java.util.Map&lt;String, String&gt;,java.lang.String,java.lang.String)</t>
   </si>
   <si>
     <t>deleteRequest(java.lang.String,java.lang.String)</t>
   </si>
   <si>
-    <t>Perform HTTP Delete request with a given path parameter</t>
-  </si>
-  <si>
-    <t>deleteRequestWithPathParameter(java.lang.String,java.lang.String,java.lang.String,java.lang.String)</t>
-  </si>
-  <si>
     <t>deleteRequestWithMultiplePathParameters(java.lang.String,java.util.Map&lt;String, String&gt;,java.lang.String)</t>
   </si>
   <si>
-    <t>APIValidationActions</t>
-  </si>
-  <si>
     <t>Get the value from JSON response</t>
   </si>
   <si>
-    <t>printAllHeaders(io.restassured.response.Response)</t>
-  </si>
-  <si>
-    <t>Print all header names and values</t>
-  </si>
-  <si>
     <t>Validate the ContentType from the response</t>
   </si>
   <si>
@@ -1070,6 +1029,51 @@
   </si>
   <si>
     <t>Mock geolocation based on latitude, longitude and accuracy</t>
+  </si>
+  <si>
+    <t>APIValidations</t>
+  </si>
+  <si>
+    <t>getRequest(java.lang.String,java.util.Map&lt;String, String&gt;,java.lang.String)</t>
+  </si>
+  <si>
+    <t>Perform HTTP Put request with query parameters and in-line body data</t>
+  </si>
+  <si>
+    <t>Perform HTTP Delete request with multiple query parameters</t>
+  </si>
+  <si>
+    <t>validateArrayListInResponse(io.restassured.response.Response, java.lang.String, java.lang.String,java.util.ArrayList&lt;String&gt;)</t>
+  </si>
+  <si>
+    <t>Validate the response array list, the expected array list values can be read from the JSON file that available at /src/test/resources/APITesting/ResponseData/ location using getArrayValuesFromJSONFile() method</t>
+  </si>
+  <si>
+    <t>validateResponseBody(io.restassured.response.Response,java.lang.String)</t>
+  </si>
+  <si>
+    <t>Validate response entire body</t>
+  </si>
+  <si>
+    <t>validateInResponseBody(io.restassured.response.Response,java.lang.String)</t>
+  </si>
+  <si>
+    <t>Validate data in the response body</t>
+  </si>
+  <si>
+    <t>Validate response data from JSON response</t>
+  </si>
+  <si>
+    <t>validateResponseData(io.restassured.response.Response,java.lang.String,java.lang.String)</t>
+  </si>
+  <si>
+    <t>APIUtilities</t>
+  </si>
+  <si>
+    <t>getArrayValuesFromJSONFile(java.lang.String,java.lang.String,java.lang.String)</t>
+  </si>
+  <si>
+    <t>Get array values from JSON file - specify the response JSON file in /src/test/resources/APITesting/ResponseData/ folder and pass the JSONFileName</t>
   </si>
 </sst>
 </file>
@@ -1690,6 +1694,67 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Left Arrow 1">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11982450" y="9525"/>
+          <a:ext cx="409575" cy="171450"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-IN" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
@@ -1746,7 +1811,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1807,7 +1872,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing13.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2300,13 +2365,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
+      <xdr:colOff>104775</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
+      <xdr:colOff>514350</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
@@ -2319,7 +2384,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11982450" y="9525"/>
+          <a:off x="12020550" y="9525"/>
           <a:ext cx="409575" cy="171450"/>
         </a:xfrm>
         <a:prstGeom prst="leftArrow">
@@ -2643,10 +2708,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:D16"/>
+  <dimension ref="C2:D17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2699,20 +2764,20 @@
         <v>288</v>
       </c>
       <c r="D8" s="28">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="3:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="26" t="s">
-        <v>315</v>
+        <v>334</v>
       </c>
       <c r="D9" s="28">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="3:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="26" t="s">
-        <v>8</v>
+        <v>346</v>
       </c>
       <c r="D10" s="28">
         <v>2</v>
@@ -2720,7 +2785,7 @@
     </row>
     <row r="11" spans="3:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="26" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D11" s="28">
         <v>2</v>
@@ -2728,42 +2793,50 @@
     </row>
     <row r="12" spans="3:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="26" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D12" s="28">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="3:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D13" s="28">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="3:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D14" s="28">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="3:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="3:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="28">
+      <c r="D16" s="28">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="27" t="s">
+    <row r="17" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="27" t="s">
         <v>175</v>
       </c>
-      <c r="D16" s="25">
-        <f>SUM(D4:D15)</f>
+      <c r="D17" s="25">
+        <f>SUM(D4:D16)</f>
         <v>167</v>
       </c>
     </row>
@@ -2776,14 +2849,15 @@
     <hyperlink ref="C5" location="UtilityActions!A1" display="UtilityActions"/>
     <hyperlink ref="C6" location="ValidationActions!A1" display="ValidationActions"/>
     <hyperlink ref="C7" location="WebActions!A1" display="WebActions"/>
-    <hyperlink ref="C10" location="AutomationEngine!A1" display="AutomationEngine"/>
-    <hyperlink ref="C11" location="CSVDataHandler!A1" display="CSVDataHandler"/>
-    <hyperlink ref="C12" location="ExcelDataHandler!A1" display="ExcelDataHandler"/>
-    <hyperlink ref="C13" location="PropertyDataHandler!A1" display="PropertyDataHandler"/>
-    <hyperlink ref="C14" location="DatabaseActions!A1" display="DatabaseActions"/>
-    <hyperlink ref="C15" location="AutomationReport!A1" display="AutomationReport"/>
+    <hyperlink ref="C11" location="AutomationEngine!A1" display="AutomationEngine"/>
+    <hyperlink ref="C12" location="CSVDataHandler!A1" display="CSVDataHandler"/>
+    <hyperlink ref="C13" location="ExcelDataHandler!A1" display="ExcelDataHandler"/>
+    <hyperlink ref="C14" location="PropertyDataHandler!A1" display="PropertyDataHandler"/>
+    <hyperlink ref="C15" location="DatabaseActions!A1" display="DatabaseActions"/>
+    <hyperlink ref="C16" location="AutomationReport!A1" display="AutomationReport"/>
     <hyperlink ref="C8" location="APIActions!A1" display="APIActions"/>
-    <hyperlink ref="C9" location="APIValidationActions!A1" display="APIValidationActions"/>
+    <hyperlink ref="C9" location="APIValidations!A1" display="APIValidations"/>
+    <hyperlink ref="C10" location="APIUtilities!A1" display="APIUtilities"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2791,6 +2865,156 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="3" max="3" width="93.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="56.42578125" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="16">
+        <v>1</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="16">
+        <v>2</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="16">
+        <v>3</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="16">
+        <v>4</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="16">
+        <v>5</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="16">
+        <v>6</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="16">
+        <v>7</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="17">
+        <v>8</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>150</v>
+      </c>
+      <c r="D9" s="31" t="s">
+        <v>157</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -2856,7 +3080,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -2908,7 +3132,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -2974,7 +3198,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -3481,10 +3705,10 @@
         <v>5</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>340</v>
+        <v>326</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>341</v>
+        <v>327</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -3747,10 +3971,10 @@
         <v>5</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>346</v>
+        <v>332</v>
       </c>
       <c r="D32" s="20" t="s">
-        <v>347</v>
+        <v>333</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -3943,10 +4167,10 @@
         <v>5</v>
       </c>
       <c r="C46" s="21" t="s">
-        <v>342</v>
+        <v>328</v>
       </c>
       <c r="D46" s="20" t="s">
-        <v>343</v>
+        <v>329</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -3957,10 +4181,10 @@
         <v>5</v>
       </c>
       <c r="C47" s="21" t="s">
-        <v>344</v>
+        <v>330</v>
       </c>
       <c r="D47" s="20" t="s">
-        <v>345</v>
+        <v>331</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -5010,11 +5234,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5049,7 +5273,7 @@
       <c r="C2" s="19" t="s">
         <v>289</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="20" t="s">
         <v>290</v>
       </c>
     </row>
@@ -5063,7 +5287,7 @@
       <c r="C3" s="19" t="s">
         <v>292</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="20" t="s">
         <v>293</v>
       </c>
     </row>
@@ -5075,9 +5299,9 @@
         <v>288</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>295</v>
-      </c>
-      <c r="D4" s="19" t="s">
+        <v>335</v>
+      </c>
+      <c r="D4" s="20" t="s">
         <v>294</v>
       </c>
     </row>
@@ -5091,11 +5315,11 @@
       <c r="C5" s="19" t="s">
         <v>299</v>
       </c>
-      <c r="D5" s="19" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D5" s="20" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="16">
         <v>5</v>
       </c>
@@ -5103,10 +5327,10 @@
         <v>288</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>300</v>
-      </c>
-      <c r="D6" s="19" t="s">
         <v>297</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -5117,10 +5341,10 @@
         <v>288</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>301</v>
+        <v>300</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -5131,10 +5355,10 @@
         <v>288</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>304</v>
-      </c>
-      <c r="D8" s="19" t="s">
-        <v>302</v>
+        <v>301</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -5145,80 +5369,24 @@
         <v>288</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>307</v>
-      </c>
-      <c r="D9" s="19" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="16">
+        <v>302</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="17">
         <v>9</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="22" t="s">
         <v>288</v>
       </c>
-      <c r="C10" s="19" t="s">
-        <v>308</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="15">
-        <v>10</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>288</v>
-      </c>
-      <c r="C11" s="19" t="s">
-        <v>310</v>
-      </c>
-      <c r="D11" s="19" t="s">
+      <c r="C10" s="22" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="16">
-        <v>11</v>
-      </c>
-      <c r="B12" s="19" t="s">
-        <v>288</v>
-      </c>
-      <c r="C12" s="19" t="s">
-        <v>311</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="15">
-        <v>12</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>288</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>314</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="16">
-        <v>13</v>
-      </c>
-      <c r="B14" s="19" t="s">
-        <v>288</v>
-      </c>
-      <c r="C14" s="19" t="s">
-        <v>313</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>312</v>
+      <c r="D10" s="23" t="s">
+        <v>337</v>
       </c>
     </row>
   </sheetData>
@@ -5233,11 +5401,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
+      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5262,18 +5430,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="38">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>315</v>
+        <v>334</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>324</v>
+        <v>338</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>316</v>
+        <v>339</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -5281,13 +5449,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>315</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>317</v>
+        <v>334</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>309</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>318</v>
+        <v>305</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -5295,13 +5463,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>315</v>
+        <v>334</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>323</v>
+        <v>308</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>319</v>
+        <v>307</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -5309,13 +5477,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>315</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>322</v>
+        <v>334</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>311</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -5323,13 +5491,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>315</v>
+        <v>334</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>325</v>
+        <v>313</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>326</v>
+        <v>314</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -5337,13 +5505,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>315</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>327</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -5351,13 +5519,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>315</v>
+        <v>334</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>330</v>
+        <v>319</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>329</v>
+        <v>317</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -5365,13 +5533,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>315</v>
+        <v>334</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>333</v>
+        <v>320</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>331</v>
+        <v>318</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -5379,13 +5547,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>315</v>
+        <v>334</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>334</v>
+        <v>340</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>332</v>
+        <v>341</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -5393,13 +5561,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>315</v>
+        <v>334</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>335</v>
+        <v>342</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>320</v>
+        <v>343</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -5407,27 +5575,55 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>315</v>
+        <v>334</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>337</v>
+        <v>345</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="39">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="38">
         <v>12</v>
       </c>
-      <c r="B13" s="33" t="s">
-        <v>315</v>
-      </c>
-      <c r="C13" s="33" t="s">
-        <v>338</v>
-      </c>
-      <c r="D13" s="31" t="s">
-        <v>339</v>
+      <c r="B13" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="38">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="38">
+        <v>14</v>
+      </c>
+      <c r="B15" s="33" t="s">
+        <v>334</v>
+      </c>
+      <c r="C15" s="33" t="s">
+        <v>324</v>
+      </c>
+      <c r="D15" s="31" t="s">
+        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -5442,11 +5638,11 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5457,130 +5653,46 @@
     <col min="4" max="4" width="56.42578125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="37" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="16">
+      <c r="A2" s="38">
         <v>1</v>
       </c>
-      <c r="B2" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>144</v>
+      <c r="B2" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>310</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="16">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="38">
         <v>2</v>
       </c>
-      <c r="B3" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>148</v>
+      <c r="B3" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>347</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="16">
-        <v>3</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="16">
-        <v>4</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="16">
-        <v>5</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="16">
-        <v>6</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="16">
-        <v>7</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="17">
-        <v>8</v>
-      </c>
-      <c r="B9" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="33" t="s">
-        <v>150</v>
-      </c>
-      <c r="D9" s="31" t="s">
-        <v>157</v>
+        <v>348</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added startLighthouseAudit to the keyword document.
</commit_message>
<xml_diff>
--- a/src/main/resources/keywords/snj-selenium-java-keywords.xlsx
+++ b/src/main/resources/keywords/snj-selenium-java-keywords.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="351">
   <si>
     <t>Keywords</t>
   </si>
@@ -1074,6 +1074,12 @@
   </si>
   <si>
     <t>Get array values from JSON file - specify the response JSON file in /src/test/resources/APITesting/ResponseData/ folder and pass the JSONFileName</t>
+  </si>
+  <si>
+    <t>startLighthouseAudit(java.lang.String,java.lang.String,java.lang.String)</t>
+  </si>
+  <si>
+    <t>Start the lighthouse audit process with different categories. Make sure that you installed the lighthouse node module package on your system using the command: npm install -g lighthouse</t>
   </si>
 </sst>
 </file>
@@ -2711,7 +2717,7 @@
   <dimension ref="C2:D17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2740,7 +2746,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="28">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="3:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -2837,7 +2843,7 @@
       </c>
       <c r="D17" s="25">
         <f>SUM(D4:D16)</f>
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -3514,11 +3520,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D53"/>
+  <dimension ref="A1:D54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4187,7 +4193,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A48" s="38">
         <v>47</v>
       </c>
@@ -4195,10 +4201,10 @@
         <v>5</v>
       </c>
       <c r="C48" s="21" t="s">
-        <v>75</v>
+        <v>349</v>
       </c>
       <c r="D48" s="20" t="s">
-        <v>217</v>
+        <v>350</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4209,10 +4215,10 @@
         <v>5</v>
       </c>
       <c r="C49" s="21" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="D49" s="20" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4223,10 +4229,10 @@
         <v>5</v>
       </c>
       <c r="C50" s="21" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="D50" s="20" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4237,10 +4243,10 @@
         <v>5</v>
       </c>
       <c r="C51" s="21" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="D51" s="20" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4250,24 +4256,38 @@
       <c r="B52" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C52" s="19" t="s">
+      <c r="C52" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="D52" s="20" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" s="38">
+        <v>52</v>
+      </c>
+      <c r="B53" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="D52" s="20" t="s">
+      <c r="D53" s="20" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="39">
-        <v>52</v>
-      </c>
-      <c r="B53" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="C53" s="32" t="s">
+    <row r="54" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="39">
+        <v>53</v>
+      </c>
+      <c r="B54" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="C54" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="D53" s="23" t="s">
+      <c r="D54" s="23" t="s">
         <v>220</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated **snj-selenium-java-keywords** document file.
</commit_message>
<xml_diff>
--- a/src/main/resources/keywords/snj-selenium-java-keywords.xlsx
+++ b/src/main/resources/keywords/snj-selenium-java-keywords.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="353">
   <si>
     <t>Keywords</t>
   </si>
@@ -1080,6 +1080,12 @@
   </si>
   <si>
     <t>Start the lighthouse audit process with different categories. Make sure that you installed the lighthouse node module package on your system using the command: npm install -g lighthouse</t>
+  </si>
+  <si>
+    <t>startAccessibilityAudit(java.lang.String,java.lang.String)</t>
+  </si>
+  <si>
+    <t>To track the violations using AxeBuilder support as part of the Accessibility Audit</t>
   </si>
 </sst>
 </file>
@@ -2716,9 +2722,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:D17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2746,7 +2750,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="28">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="3:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -2843,7 +2847,7 @@
       </c>
       <c r="D17" s="25">
         <f>SUM(D4:D16)</f>
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -3520,11 +3524,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D54"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C48" sqref="C48"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4215,10 +4219,10 @@
         <v>5</v>
       </c>
       <c r="C49" s="21" t="s">
-        <v>75</v>
+        <v>351</v>
       </c>
       <c r="D49" s="20" t="s">
-        <v>217</v>
+        <v>352</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4229,10 +4233,10 @@
         <v>5</v>
       </c>
       <c r="C50" s="21" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="D50" s="20" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4243,10 +4247,10 @@
         <v>5</v>
       </c>
       <c r="C51" s="21" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="D51" s="20" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4257,10 +4261,10 @@
         <v>5</v>
       </c>
       <c r="C52" s="21" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="D52" s="20" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4270,24 +4274,38 @@
       <c r="B53" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C53" s="19" t="s">
+      <c r="C53" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="D53" s="20" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54" s="38">
+        <v>53</v>
+      </c>
+      <c r="B54" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C54" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="D53" s="20" t="s">
+      <c r="D54" s="20" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="39">
-        <v>53</v>
-      </c>
-      <c r="B54" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="C54" s="32" t="s">
+    <row r="55" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="39">
+        <v>54</v>
+      </c>
+      <c r="B55" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="C55" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="D54" s="23" t="s">
+      <c r="D55" s="23" t="s">
         <v>220</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated the snj-selenium-java keyword document.
</commit_message>
<xml_diff>
--- a/src/main/resources/keywords/snj-selenium-java-keywords.xlsx
+++ b/src/main/resources/keywords/snj-selenium-java-keywords.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="361">
   <si>
     <t>Keywords</t>
   </si>
@@ -1086,6 +1086,30 @@
   </si>
   <si>
     <t>To track the violations using AxeBuilder support as part of the Accessibility Audit</t>
+  </si>
+  <si>
+    <t>waitForElement(org.openqa.selenium.WebDriver,java.lang.String, long)</t>
+  </si>
+  <si>
+    <t>Wait for the element using the object mentioned in the Object repository</t>
+  </si>
+  <si>
+    <t>getLongWaitingTime()</t>
+  </si>
+  <si>
+    <t>getShortWaitingTime()</t>
+  </si>
+  <si>
+    <t>Get the long waiting time from the framework config file</t>
+  </si>
+  <si>
+    <t>Get the short waiting time from the framework config file</t>
+  </si>
+  <si>
+    <t>collectLoadTime(org.openqa.selenium.WebDriver,java.lang.String,long,java.lang.String, ,java.lang.String)</t>
+  </si>
+  <si>
+    <t>Collect the page load time during automation execution</t>
   </si>
 </sst>
 </file>
@@ -2722,7 +2746,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:D17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2750,7 +2776,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="28">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="3:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -2847,7 +2873,7 @@
       </c>
       <c r="D17" s="25">
         <f>SUM(D4:D16)</f>
-        <v>169</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -3524,11 +3550,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D55"/>
+  <dimension ref="A1:D59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C49" sqref="C49"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4232,11 +4258,11 @@
       <c r="B50" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C50" s="21" t="s">
-        <v>75</v>
+      <c r="C50" s="19" t="s">
+        <v>359</v>
       </c>
       <c r="D50" s="20" t="s">
-        <v>217</v>
+        <v>360</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4247,10 +4273,10 @@
         <v>5</v>
       </c>
       <c r="C51" s="21" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="D51" s="20" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4261,10 +4287,10 @@
         <v>5</v>
       </c>
       <c r="C52" s="21" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="D52" s="20" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4275,10 +4301,10 @@
         <v>5</v>
       </c>
       <c r="C53" s="21" t="s">
-        <v>66</v>
+        <v>353</v>
       </c>
       <c r="D53" s="20" t="s">
-        <v>221</v>
+        <v>354</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4288,25 +4314,81 @@
       <c r="B54" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C54" s="19" t="s">
+      <c r="C54" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="D54" s="20" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A55" s="38">
+        <v>54</v>
+      </c>
+      <c r="B55" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C55" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="D55" s="20" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56" s="38">
+        <v>55</v>
+      </c>
+      <c r="B56" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C56" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="D54" s="20" t="s">
+      <c r="D56" s="20" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="39">
-        <v>54</v>
-      </c>
-      <c r="B55" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="C55" s="32" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="38">
+        <v>56</v>
+      </c>
+      <c r="B57" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C57" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="D55" s="23" t="s">
+      <c r="D57" s="20" t="s">
         <v>220</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="38">
+        <v>57</v>
+      </c>
+      <c r="B58" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C58" s="19" t="s">
+        <v>355</v>
+      </c>
+      <c r="D58" s="20" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="39">
+        <v>58</v>
+      </c>
+      <c r="B59" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="C59" s="32" t="s">
+        <v>356</v>
+      </c>
+      <c r="D59" s="23" t="s">
+        <v>358</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the keyword document snj-selenium-java-keywords.
</commit_message>
<xml_diff>
--- a/src/main/resources/keywords/snj-selenium-java-keywords.xlsx
+++ b/src/main/resources/keywords/snj-selenium-java-keywords.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="377">
   <si>
     <t>Keywords</t>
   </si>
@@ -1122,6 +1122,42 @@
   </si>
   <si>
     <t>verifyJSONContent(java.lang.String,java.lang.String)</t>
+  </si>
+  <si>
+    <t>getParameterValueFromTestNG(java.lang.String)</t>
+  </si>
+  <si>
+    <t>getParameterValueFromTestNG(java.lang.String, java.lang.String)</t>
+  </si>
+  <si>
+    <t>Read parameter value based on the given testng.xml file and key name</t>
+  </si>
+  <si>
+    <t>Read parameter value based on the given key name from the testng.xml file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">compareImages(org.openqa.selenium.WebDriver,java.lang.String,java.lang.String,java.lang.String) </t>
+  </si>
+  <si>
+    <t>Capture the current screen and compare it with expected image file</t>
+  </si>
+  <si>
+    <t xml:space="preserve">compareImages(java.lang.String,java.lang.String) </t>
+  </si>
+  <si>
+    <t>Compares two images that send by the user and will return the percentage value for assertion</t>
+  </si>
+  <si>
+    <t>startRecording(java.lang.String)</t>
+  </si>
+  <si>
+    <t>stopRecording()</t>
+  </si>
+  <si>
+    <t>Start video recording and store it in Automation_Videos folder inside Reports folder</t>
+  </si>
+  <si>
+    <t>Stop video recording</t>
   </si>
 </sst>
 </file>
@@ -2759,7 +2795,7 @@
   <dimension ref="C2:D17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2788,7 +2824,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="28">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="3:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -2796,7 +2832,7 @@
         <v>6</v>
       </c>
       <c r="D6" s="28">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="3:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -2885,7 +2921,7 @@
       </c>
       <c r="D17" s="25">
         <f>SUM(D4:D16)</f>
-        <v>175</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -3318,7 +3354,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3562,11 +3598,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D59"/>
+  <dimension ref="A1:D63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3711,38 +3747,38 @@
         <v>5</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>40</v>
+        <v>365</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="38">
         <v>10</v>
       </c>
       <c r="B11" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="21" t="s">
-        <v>86</v>
+      <c r="C11" s="19" t="s">
+        <v>366</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="38">
         <v>11</v>
       </c>
       <c r="B12" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="21" t="s">
-        <v>85</v>
+      <c r="C12" s="19" t="s">
+        <v>40</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -3753,10 +3789,10 @@
         <v>5</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>326</v>
+        <v>86</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>327</v>
+        <v>185</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -3767,10 +3803,10 @@
         <v>5</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -3781,10 +3817,10 @@
         <v>5</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>64</v>
+        <v>326</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>188</v>
+        <v>327</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -3795,10 +3831,10 @@
         <v>5</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -3808,11 +3844,11 @@
       <c r="B17" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="19" t="s">
-        <v>51</v>
+      <c r="C17" s="21" t="s">
+        <v>64</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -3823,10 +3859,10 @@
         <v>5</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -3836,11 +3872,11 @@
       <c r="B19" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="21" t="s">
-        <v>56</v>
+      <c r="C19" s="19" t="s">
+        <v>51</v>
       </c>
       <c r="D19" s="20" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -3850,11 +3886,11 @@
       <c r="B20" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="19" t="s">
-        <v>42</v>
+      <c r="C20" s="21" t="s">
+        <v>58</v>
       </c>
       <c r="D20" s="20" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -3864,11 +3900,11 @@
       <c r="B21" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="19" t="s">
-        <v>43</v>
+      <c r="C21" s="21" t="s">
+        <v>56</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -3878,11 +3914,11 @@
       <c r="B22" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="21" t="s">
-        <v>63</v>
+      <c r="C22" s="19" t="s">
+        <v>42</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -3893,10 +3929,10 @@
         <v>5</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -3906,11 +3942,11 @@
       <c r="B24" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C24" s="19" t="s">
-        <v>45</v>
+      <c r="C24" s="21" t="s">
+        <v>63</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -3920,14 +3956,14 @@
       <c r="B25" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="21" t="s">
-        <v>82</v>
+      <c r="C25" s="19" t="s">
+        <v>48</v>
       </c>
       <c r="D25" s="20" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="38">
         <v>25</v>
       </c>
@@ -3935,10 +3971,10 @@
         <v>5</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -3949,10 +3985,10 @@
         <v>5</v>
       </c>
       <c r="C27" s="21" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3962,14 +3998,14 @@
       <c r="B28" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C28" s="21" t="s">
-        <v>77</v>
+      <c r="C28" s="19" t="s">
+        <v>49</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="38">
         <v>28</v>
       </c>
@@ -3977,10 +4013,10 @@
         <v>5</v>
       </c>
       <c r="C29" s="21" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3991,10 +4027,10 @@
         <v>5</v>
       </c>
       <c r="C30" s="21" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="D30" s="20" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4004,56 +4040,56 @@
       <c r="B31" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="19" t="s">
-        <v>270</v>
+      <c r="C31" s="21" t="s">
+        <v>59</v>
       </c>
       <c r="D31" s="20" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="38">
         <v>31</v>
       </c>
       <c r="B32" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C32" s="19" t="s">
-        <v>332</v>
+      <c r="C32" s="21" t="s">
+        <v>60</v>
       </c>
       <c r="D32" s="20" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="38">
         <v>32</v>
       </c>
       <c r="B33" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C33" s="21" t="s">
-        <v>67</v>
+      <c r="C33" s="19" t="s">
+        <v>270</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="38">
         <v>33</v>
       </c>
       <c r="B34" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C34" s="21" t="s">
-        <v>68</v>
+      <c r="C34" s="19" t="s">
+        <v>332</v>
       </c>
       <c r="D34" s="20" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="38">
         <v>34</v>
       </c>
@@ -4061,13 +4097,13 @@
         <v>5</v>
       </c>
       <c r="C35" s="21" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="D35" s="20" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="38">
         <v>35</v>
       </c>
@@ -4075,13 +4111,13 @@
         <v>5</v>
       </c>
       <c r="C36" s="21" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D36" s="20" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="38">
         <v>36</v>
       </c>
@@ -4089,10 +4125,10 @@
         <v>5</v>
       </c>
       <c r="C37" s="21" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="D37" s="20" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -4103,10 +4139,10 @@
         <v>5</v>
       </c>
       <c r="C38" s="21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D38" s="20" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -4117,10 +4153,10 @@
         <v>5</v>
       </c>
       <c r="C39" s="21" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D39" s="20" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -4131,10 +4167,10 @@
         <v>5</v>
       </c>
       <c r="C40" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D40" s="20" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -4144,11 +4180,11 @@
       <c r="B41" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C41" s="19" t="s">
-        <v>52</v>
+      <c r="C41" s="21" t="s">
+        <v>74</v>
       </c>
       <c r="D41" s="20" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -4158,11 +4194,11 @@
       <c r="B42" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C42" s="19" t="s">
-        <v>46</v>
+      <c r="C42" s="21" t="s">
+        <v>73</v>
       </c>
       <c r="D42" s="20" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -4173,13 +4209,13 @@
         <v>5</v>
       </c>
       <c r="C43" s="19" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="D43" s="20" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="38">
         <v>43</v>
       </c>
@@ -4187,41 +4223,41 @@
         <v>5</v>
       </c>
       <c r="C44" s="19" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D44" s="20" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="38">
         <v>44</v>
       </c>
       <c r="B45" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C45" s="21" t="s">
-        <v>57</v>
+      <c r="C45" s="19" t="s">
+        <v>47</v>
       </c>
       <c r="D45" s="20" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="38">
         <v>45</v>
       </c>
       <c r="B46" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C46" s="21" t="s">
-        <v>328</v>
+      <c r="C46" s="19" t="s">
+        <v>50</v>
       </c>
       <c r="D46" s="20" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="38">
         <v>46</v>
       </c>
@@ -4229,13 +4265,13 @@
         <v>5</v>
       </c>
       <c r="C47" s="21" t="s">
-        <v>330</v>
+        <v>57</v>
       </c>
       <c r="D47" s="20" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="38">
         <v>47</v>
       </c>
@@ -4243,13 +4279,13 @@
         <v>5</v>
       </c>
       <c r="C48" s="21" t="s">
-        <v>349</v>
+        <v>328</v>
       </c>
       <c r="D48" s="20" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="38">
         <v>48</v>
       </c>
@@ -4257,24 +4293,24 @@
         <v>5</v>
       </c>
       <c r="C49" s="21" t="s">
-        <v>351</v>
+        <v>330</v>
       </c>
       <c r="D49" s="20" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A50" s="38">
         <v>49</v>
       </c>
       <c r="B50" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C50" s="19" t="s">
-        <v>359</v>
+      <c r="C50" s="21" t="s">
+        <v>349</v>
       </c>
       <c r="D50" s="20" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4285,10 +4321,10 @@
         <v>5</v>
       </c>
       <c r="C51" s="21" t="s">
-        <v>75</v>
+        <v>351</v>
       </c>
       <c r="D51" s="20" t="s">
-        <v>217</v>
+        <v>352</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4298,11 +4334,11 @@
       <c r="B52" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C52" s="21" t="s">
-        <v>61</v>
+      <c r="C52" s="19" t="s">
+        <v>359</v>
       </c>
       <c r="D52" s="20" t="s">
-        <v>218</v>
+        <v>360</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4312,25 +4348,25 @@
       <c r="B53" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C53" s="21" t="s">
-        <v>353</v>
+      <c r="C53" s="19" t="s">
+        <v>373</v>
       </c>
       <c r="D53" s="20" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="38">
         <v>53</v>
       </c>
       <c r="B54" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C54" s="21" t="s">
-        <v>55</v>
+      <c r="C54" s="19" t="s">
+        <v>374</v>
       </c>
       <c r="D54" s="20" t="s">
-        <v>219</v>
+        <v>376</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4341,10 +4377,10 @@
         <v>5</v>
       </c>
       <c r="C55" s="21" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="D55" s="20" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4354,14 +4390,14 @@
       <c r="B56" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C56" s="19" t="s">
-        <v>44</v>
+      <c r="C56" s="21" t="s">
+        <v>61</v>
       </c>
       <c r="D56" s="20" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="38">
         <v>56</v>
       </c>
@@ -4369,37 +4405,93 @@
         <v>5</v>
       </c>
       <c r="C57" s="21" t="s">
-        <v>62</v>
+        <v>353</v>
       </c>
       <c r="D57" s="20" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="38">
         <v>57</v>
       </c>
       <c r="B58" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C58" s="19" t="s">
+      <c r="C58" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="D58" s="20" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" s="38">
+        <v>58</v>
+      </c>
+      <c r="B59" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C59" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="D59" s="20" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A60" s="38">
+        <v>59</v>
+      </c>
+      <c r="B60" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C60" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="D60" s="20" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="38">
+        <v>60</v>
+      </c>
+      <c r="B61" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C61" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="D61" s="20" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="38">
+        <v>61</v>
+      </c>
+      <c r="B62" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C62" s="19" t="s">
         <v>355</v>
       </c>
-      <c r="D58" s="20" t="s">
+      <c r="D62" s="20" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="39">
-        <v>58</v>
-      </c>
-      <c r="B59" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="C59" s="32" t="s">
+    <row r="63" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="39">
+        <v>62</v>
+      </c>
+      <c r="B63" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="C63" s="32" t="s">
         <v>356</v>
       </c>
-      <c r="D59" s="23" t="s">
+      <c r="D63" s="23" t="s">
         <v>358</v>
       </c>
     </row>
@@ -4412,11 +4504,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C32" sqref="C32"/>
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4889,7 +4981,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="38">
         <v>33</v>
       </c>
@@ -4897,10 +4989,10 @@
         <v>6</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>114</v>
+        <v>369</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>245</v>
+        <v>370</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4911,13 +5003,13 @@
         <v>6</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>104</v>
+        <v>371</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="38">
         <v>35</v>
       </c>
@@ -4925,23 +5017,51 @@
         <v>6</v>
       </c>
       <c r="C36" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="38">
+        <v>36</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="38">
+        <v>37</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="D36" s="6" t="s">
+      <c r="D38" s="6" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="39">
-        <v>36</v>
-      </c>
-      <c r="B37" s="33" t="s">
+    <row r="39" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="39">
+        <v>38</v>
+      </c>
+      <c r="B39" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="C37" s="30" t="s">
+      <c r="C39" s="30" t="s">
         <v>364</v>
       </c>
-      <c r="D37" s="31" t="s">
+      <c r="D39" s="31" t="s">
         <v>363</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added new keywords for API Utilities.
</commit_message>
<xml_diff>
--- a/src/main/resources/keywords/snj-selenium-java-keywords.xlsx
+++ b/src/main/resources/keywords/snj-selenium-java-keywords.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15030" windowHeight="7470"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="11" r:id="rId1"/>
@@ -21,11 +21,12 @@
     <sheet name="AutomationReport" sheetId="1" r:id="rId12"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <oleSize ref="A1:M19"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="412">
   <si>
     <t>Keywords</t>
   </si>
@@ -1243,6 +1244,24 @@
   </si>
   <si>
     <t>getIntegerValuesbyColNum(ResultSet resultSet, int colIndex)</t>
+  </si>
+  <si>
+    <t>updateJSONArrayNode(String JSONFilePath, String excelSheetName, String columnName, List&lt;String&gt; parentObjectList, String arrayNodeName)</t>
+  </si>
+  <si>
+    <t>Method to update the JSON Array node</t>
+  </si>
+  <si>
+    <t>updateJSONArrayNode(String JSONFilePath, String excelFilePath, String excelSheetName, String columnName, List&lt;String&gt; parentObjectList, String arrayNodeName)</t>
+  </si>
+  <si>
+    <t>Method to update the JSON Array node with excel file path</t>
+  </si>
+  <si>
+    <t>deleteJSONArrayNode(String JSONFilePath, List&lt;String&gt; parentObjectList, String arrayNodeName)</t>
+  </si>
+  <si>
+    <t>Method to delete JSON array node</t>
   </si>
 </sst>
 </file>
@@ -1705,11 +1724,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1717,7 +1733,10 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2699,7 +2718,7 @@
   <dimension ref="C2:D15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2710,10 +2729,10 @@
   <sheetData>
     <row r="2" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="3:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="37"/>
+      <c r="D3" s="36"/>
     </row>
     <row r="4" spans="3:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="22" t="s">
@@ -2768,7 +2787,7 @@
         <v>118</v>
       </c>
       <c r="D10" s="24">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="3:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -2809,7 +2828,7 @@
       </c>
       <c r="D15" s="21">
         <f>SUM(D4:D14)</f>
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -3514,7 +3533,7 @@
       <c r="B1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="34" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="31" t="s">
@@ -5756,11 +5775,11 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1:C1048576"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5772,21 +5791,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="38" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="34">
+      <c r="A2" s="37">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -5795,12 +5814,12 @@
       <c r="C2" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="34">
+      <c r="A3" s="37">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -5809,12 +5828,12 @@
       <c r="C3" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="34">
+      <c r="A4" s="37">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -5823,12 +5842,12 @@
       <c r="C4" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="34">
+      <c r="A5" s="37">
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -5837,12 +5856,12 @@
       <c r="C5" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="34">
+      <c r="A6" s="37">
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -5851,12 +5870,12 @@
       <c r="C6" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="34">
+      <c r="A7" s="37">
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -5865,12 +5884,12 @@
       <c r="C7" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="34">
+      <c r="A8" s="37">
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -5879,12 +5898,12 @@
       <c r="C8" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="5" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="34">
+      <c r="A9" s="37">
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -5893,12 +5912,12 @@
       <c r="C9" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="5" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="34">
+      <c r="A10" s="37">
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -5907,12 +5926,12 @@
       <c r="C10" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="5" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="34">
+      <c r="A11" s="37">
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -5921,12 +5940,12 @@
       <c r="C11" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="5" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="34">
+      <c r="A12" s="37">
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -5935,12 +5954,12 @@
       <c r="C12" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="5" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="34">
+      <c r="A13" s="37">
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
@@ -5949,12 +5968,12 @@
       <c r="C13" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="5" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="34">
+      <c r="A14" s="37">
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -5963,12 +5982,12 @@
       <c r="C14" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="5" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="34">
+      <c r="A15" s="37">
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
@@ -5977,22 +5996,64 @@
       <c r="C15" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="5" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="35">
+    <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="37">
         <v>15</v>
       </c>
-      <c r="B16" s="28" t="s">
+      <c r="B16" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C16" s="25" t="s">
+      <c r="C16" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="D16" s="26" t="s">
+      <c r="D16" s="5" t="s">
         <v>167</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="37">
+        <v>16</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>406</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="37">
+        <v>17</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>408</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="37">
+        <v>18</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>410</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>411</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Support for GraphQL API automation. - Updated the keyword document snj-selenium-java-keywords
</commit_message>
<xml_diff>
--- a/src/main/resources/keywords/snj-selenium-java-keywords.xlsx
+++ b/src/main/resources/keywords/snj-selenium-java-keywords.xlsx
@@ -18,14 +18,15 @@
     <sheet name="APIUtilities" sheetId="14" r:id="rId9"/>
     <sheet name="DataHandler" sheetId="8" r:id="rId10"/>
     <sheet name="AutomationEngine" sheetId="6" r:id="rId11"/>
-    <sheet name="AutomationReport" sheetId="1" r:id="rId12"/>
+    <sheet name="DataGenerator" sheetId="15" r:id="rId12"/>
+    <sheet name="AutomationReport" sheetId="1" r:id="rId13"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1163" uniqueCount="776">
   <si>
     <t>Keywords</t>
   </si>
@@ -1149,9 +1150,6 @@
     <t>verifyJSONFileContent(String expectedJSONPath, String actualJSONPath)</t>
   </si>
   <si>
-    <t>verifyFileUpload(String downloadPath, String fileName, String messageOnFailure)</t>
-  </si>
-  <si>
     <t>Verify the file downloaded or not</t>
   </si>
   <si>
@@ -1260,18 +1258,9 @@
     <t>postRequestWithBody(String baseURI, String endPointPath, String requestBody, String contentType)</t>
   </si>
   <si>
-    <t xml:space="preserve">Perform HTTP Post request with direct body data. </t>
-  </si>
-  <si>
-    <t>getRequestWithAuthToken(String baseURI, String endPointPath, String authenticationScheme, String token, String pathParamName, String pathParamValue)</t>
-  </si>
-  <si>
     <t>getRequestWithAuthToken(String baseURI, String endPointPath, String authenticationScheme, String token)</t>
   </si>
   <si>
-    <t>Perform HTTP Get request with authorization token and path parameter</t>
-  </si>
-  <si>
     <t>patchRequestWithBody(String baseURI, String endPointPath, String requestBody, String contentType)</t>
   </si>
   <si>
@@ -1281,7 +1270,1090 @@
     <t>patchRequestWithBody(String baseURI, String endPointPath, String requestBody, String authenticationScheme, String token, String contentType)</t>
   </si>
   <si>
-    <t>Perform HTTP Patch request with direct body data with token.</t>
+    <t>DataGenerator</t>
+  </si>
+  <si>
+    <t>DataGenerator.Name</t>
+  </si>
+  <si>
+    <t>getPrefix()</t>
+  </si>
+  <si>
+    <t>Method to get the prefix</t>
+  </si>
+  <si>
+    <t>getSuffix()</t>
+  </si>
+  <si>
+    <t>Method to get the suffix</t>
+  </si>
+  <si>
+    <t>getFirstName()</t>
+  </si>
+  <si>
+    <t>Method to get the first name</t>
+  </si>
+  <si>
+    <t>getFirstName(Locale locale)</t>
+  </si>
+  <si>
+    <t>Method to get the first name based on locale</t>
+  </si>
+  <si>
+    <t>getLastName()</t>
+  </si>
+  <si>
+    <t>Method to get the last name</t>
+  </si>
+  <si>
+    <t>getLastName(Locale locale)</t>
+  </si>
+  <si>
+    <t>Method to get the last name based on locale</t>
+  </si>
+  <si>
+    <t>getFullName()</t>
+  </si>
+  <si>
+    <t>Method to get the full name</t>
+  </si>
+  <si>
+    <t>getFullName(Locale locale)</t>
+  </si>
+  <si>
+    <t>Method to get the full name based on locale</t>
+  </si>
+  <si>
+    <t>getUsername()</t>
+  </si>
+  <si>
+    <t>Method to get the username</t>
+  </si>
+  <si>
+    <t>getUsername(Locale locale)</t>
+  </si>
+  <si>
+    <t>Method to get the username based on locale</t>
+  </si>
+  <si>
+    <t>DataGenerator.Address</t>
+  </si>
+  <si>
+    <t>getBuildingNumber()</t>
+  </si>
+  <si>
+    <t>Method to get the building number</t>
+  </si>
+  <si>
+    <t>getBuildingNumber(Locale locale)</t>
+  </si>
+  <si>
+    <t>Method to get the building number based on locale</t>
+  </si>
+  <si>
+    <t>getStreetAddress()</t>
+  </si>
+  <si>
+    <t>Method to get the street address</t>
+  </si>
+  <si>
+    <t>getStreetAddress(Locale locale)</t>
+  </si>
+  <si>
+    <t>Method to get the street address based on locale</t>
+  </si>
+  <si>
+    <t>getSecondaryAddress()</t>
+  </si>
+  <si>
+    <t>Method to get the secondary address</t>
+  </si>
+  <si>
+    <t>getSecondaryAddress(Locale locale)</t>
+  </si>
+  <si>
+    <t>Method to get the secondary address based on locale</t>
+  </si>
+  <si>
+    <t>getCity()</t>
+  </si>
+  <si>
+    <t>Method to get the city</t>
+  </si>
+  <si>
+    <t>getCity(Locale locale)</t>
+  </si>
+  <si>
+    <t>Method to get the city based on locale</t>
+  </si>
+  <si>
+    <t>getState()</t>
+  </si>
+  <si>
+    <t>Method to get the state</t>
+  </si>
+  <si>
+    <t>getState(Locale locale)</t>
+  </si>
+  <si>
+    <t>Method to get the state based on locale</t>
+  </si>
+  <si>
+    <t>getCountry()</t>
+  </si>
+  <si>
+    <t>Method to get the country</t>
+  </si>
+  <si>
+    <t>getCountry(Locale locale)</t>
+  </si>
+  <si>
+    <t>Method to get the country based on locale</t>
+  </si>
+  <si>
+    <t>getCountryCode()</t>
+  </si>
+  <si>
+    <t>Method to get the city code</t>
+  </si>
+  <si>
+    <t>getCountryCode(Locale locale)</t>
+  </si>
+  <si>
+    <t>Method to get the country code based on locale</t>
+  </si>
+  <si>
+    <t>getZipCode()</t>
+  </si>
+  <si>
+    <t>Method to get the zipcode</t>
+  </si>
+  <si>
+    <t>getZipCode(Locale locale)</t>
+  </si>
+  <si>
+    <t>Method to get the zipcode based on locale</t>
+  </si>
+  <si>
+    <t>getFullAddress()</t>
+  </si>
+  <si>
+    <t>Method to get the full address</t>
+  </si>
+  <si>
+    <t>getFullAddress(Locale locale)</t>
+  </si>
+  <si>
+    <t>Method to get the full address based on the locale</t>
+  </si>
+  <si>
+    <t>getTimeZone()</t>
+  </si>
+  <si>
+    <t>Method to get the time-zone</t>
+  </si>
+  <si>
+    <t>getTimeZone(Locale locale)</t>
+  </si>
+  <si>
+    <t>Method to get the time-zone based on locale</t>
+  </si>
+  <si>
+    <t>getLatitude()</t>
+  </si>
+  <si>
+    <t>Method to get latitude</t>
+  </si>
+  <si>
+    <t>getLatitude(Locale locale)</t>
+  </si>
+  <si>
+    <t>Method to get the latitude based on locale</t>
+  </si>
+  <si>
+    <t>getLongitude()</t>
+  </si>
+  <si>
+    <t>Method to get the longitude</t>
+  </si>
+  <si>
+    <t>getLongitude(Locale locale)</t>
+  </si>
+  <si>
+    <t>Method to get the longitude based on locale</t>
+  </si>
+  <si>
+    <t>getLatitudeLongitude()</t>
+  </si>
+  <si>
+    <t>Method to get the latitude-longitude</t>
+  </si>
+  <si>
+    <t>getLatitudeLongitude(Locale locale)</t>
+  </si>
+  <si>
+    <t>Method to get the latitude-longitude based on locale</t>
+  </si>
+  <si>
+    <t>DataGenerator.Phone</t>
+  </si>
+  <si>
+    <t>getCellPhone()</t>
+  </si>
+  <si>
+    <t>Method to get the cell phone</t>
+  </si>
+  <si>
+    <t>getCellPhone(Locale locale)</t>
+  </si>
+  <si>
+    <t>Method to get the cell phone based on locale</t>
+  </si>
+  <si>
+    <t>getPhoneNumber()</t>
+  </si>
+  <si>
+    <t>Method to get the phone number</t>
+  </si>
+  <si>
+    <t>getPhoneNumber(Locale locale)</t>
+  </si>
+  <si>
+    <t>Method to get the phone number based on locale</t>
+  </si>
+  <si>
+    <t>DataGenerator.Appliance</t>
+  </si>
+  <si>
+    <t>getBrand()</t>
+  </si>
+  <si>
+    <t>Method to get the brand name</t>
+  </si>
+  <si>
+    <t>getBrand(Locale locale)</t>
+  </si>
+  <si>
+    <t>Method to get the brand name based on locale</t>
+  </si>
+  <si>
+    <t>getEquipment()</t>
+  </si>
+  <si>
+    <t>Method to get the equipment name</t>
+  </si>
+  <si>
+    <t>getEquipment(Locale locale)</t>
+  </si>
+  <si>
+    <t>Method to get the equipment name based on locale</t>
+  </si>
+  <si>
+    <t>DataGenerator.Artist</t>
+  </si>
+  <si>
+    <t>getArtistName()</t>
+  </si>
+  <si>
+    <t>Method to get the artist name</t>
+  </si>
+  <si>
+    <t>getArtistName(Locale locale)</t>
+  </si>
+  <si>
+    <t>Method to get the artist name based on locale</t>
+  </si>
+  <si>
+    <t>DataGenerator.Avatar</t>
+  </si>
+  <si>
+    <t>getAvatar()</t>
+  </si>
+  <si>
+    <t>Method to get the avatar image as link</t>
+  </si>
+  <si>
+    <t>DataGenerator.Aviation</t>
+  </si>
+  <si>
+    <t>getAirport()</t>
+  </si>
+  <si>
+    <t>Method to get the Airport name</t>
+  </si>
+  <si>
+    <t>getAirport(Locale locale)</t>
+  </si>
+  <si>
+    <t>Method to get the Airport name based on locale</t>
+  </si>
+  <si>
+    <t>getAircraft()</t>
+  </si>
+  <si>
+    <t>Method to get the Aircraft name</t>
+  </si>
+  <si>
+    <t>getAircraft(Locale locale)</t>
+  </si>
+  <si>
+    <t>Method to get the Aircraft name based on locale</t>
+  </si>
+  <si>
+    <t>getAirline()</t>
+  </si>
+  <si>
+    <t>Method to get the Airline name</t>
+  </si>
+  <si>
+    <t>getAirline(Locale locale)</t>
+  </si>
+  <si>
+    <t>Method to get the Airline name based on locale</t>
+  </si>
+  <si>
+    <t>getFlight()</t>
+  </si>
+  <si>
+    <t>Method to get the flight name</t>
+  </si>
+  <si>
+    <t>getFlight(Locale locale)</t>
+  </si>
+  <si>
+    <t>Method to get the flight name based on locale</t>
+  </si>
+  <si>
+    <t>DataGenerator.Barcode</t>
+  </si>
+  <si>
+    <t>getBarcodeType()</t>
+  </si>
+  <si>
+    <t>Method to get the barcode type</t>
+  </si>
+  <si>
+    <t>getBarcode(String ean_gtin)</t>
+  </si>
+  <si>
+    <t>Method to get the barcode based on ean or gtin number, it can be ean13 or ean8 or gtin8 or gtin12 or gtin13 or gtin14</t>
+  </si>
+  <si>
+    <t>DataGenerator.Book</t>
+  </si>
+  <si>
+    <t>getBookTitle()</t>
+  </si>
+  <si>
+    <t>Method to get the book title</t>
+  </si>
+  <si>
+    <t>getBookTitle(Locale locale)</t>
+  </si>
+  <si>
+    <t>Method to get the book title based on locale</t>
+  </si>
+  <si>
+    <t>getAuthor()</t>
+  </si>
+  <si>
+    <t>Method to get the author name</t>
+  </si>
+  <si>
+    <t>getAuthor(Locale locale)</t>
+  </si>
+  <si>
+    <t>Method to get the author name based on locale</t>
+  </si>
+  <si>
+    <t>getGenre()</t>
+  </si>
+  <si>
+    <t>Method to get the genre name</t>
+  </si>
+  <si>
+    <t>getPublisher()</t>
+  </si>
+  <si>
+    <t>Method to get the publisher name</t>
+  </si>
+  <si>
+    <t>getPublisher(Locale locale)</t>
+  </si>
+  <si>
+    <t>Method to get the publisher name based on locale</t>
+  </si>
+  <si>
+    <t>DataGenerator.Brand</t>
+  </si>
+  <si>
+    <t>getCarBrand()</t>
+  </si>
+  <si>
+    <t>Method to get the car brand</t>
+  </si>
+  <si>
+    <t>getCarBrand(Locale locale)</t>
+  </si>
+  <si>
+    <t>Method to get the car brand based on locale</t>
+  </si>
+  <si>
+    <t>getWatchBrand()</t>
+  </si>
+  <si>
+    <t>Method to get the watch brand</t>
+  </si>
+  <si>
+    <t>getWatchBrand(Locale locale)</t>
+  </si>
+  <si>
+    <t>Method to get the watch brand based on locale</t>
+  </si>
+  <si>
+    <t>getSportBrand()</t>
+  </si>
+  <si>
+    <t>Method to get the sport brand</t>
+  </si>
+  <si>
+    <t>DataGenerator.BankingOrFinance</t>
+  </si>
+  <si>
+    <t>getCreditCardType()</t>
+  </si>
+  <si>
+    <t>Method to get the credit card type</t>
+  </si>
+  <si>
+    <t>getCreditCardNumber()</t>
+  </si>
+  <si>
+    <t>Method to get the credit card number</t>
+  </si>
+  <si>
+    <t>getCreditCardExpiry()</t>
+  </si>
+  <si>
+    <t>Method to get the credit card expiry</t>
+  </si>
+  <si>
+    <t>getSecurityCode()</t>
+  </si>
+  <si>
+    <t>Method to get the security code</t>
+  </si>
+  <si>
+    <t>getBusinessIdentificationCode()</t>
+  </si>
+  <si>
+    <t>Method to get the Business Identification Code</t>
+  </si>
+  <si>
+    <t>getStockMarketName()</t>
+  </si>
+  <si>
+    <t>Method to get the Stock Market Name</t>
+  </si>
+  <si>
+    <t>DataGenerator.Color</t>
+  </si>
+  <si>
+    <t>getColorName()</t>
+  </si>
+  <si>
+    <t>Method to get the name of the color</t>
+  </si>
+  <si>
+    <t>getHexColorCode()</t>
+  </si>
+  <si>
+    <t>Method to get the hex color code</t>
+  </si>
+  <si>
+    <t>getHexColorCode(boolean includeHashSign)</t>
+  </si>
+  <si>
+    <t>Method to get the hex color code based on the flag includeHashSign</t>
+  </si>
+  <si>
+    <t>DataGenerator.Commerce</t>
+  </si>
+  <si>
+    <t>getDepartmentName()</t>
+  </si>
+  <si>
+    <t>Method to get the department name</t>
+  </si>
+  <si>
+    <t>getProductBrand()</t>
+  </si>
+  <si>
+    <t>Method to get the product brand</t>
+  </si>
+  <si>
+    <t>getProductName()</t>
+  </si>
+  <si>
+    <t>Method to get the product name</t>
+  </si>
+  <si>
+    <t>getMaterial()</t>
+  </si>
+  <si>
+    <t>Method to get the material name</t>
+  </si>
+  <si>
+    <t>DataGenerator.Company</t>
+  </si>
+  <si>
+    <t>getCompanyName()</t>
+  </si>
+  <si>
+    <t>Method to get the company name</t>
+  </si>
+  <si>
+    <t>getCompanyLogo()</t>
+  </si>
+  <si>
+    <t>Method to get the company logo as link</t>
+  </si>
+  <si>
+    <t>getCompanyURL()</t>
+  </si>
+  <si>
+    <t>Method to get the company URL</t>
+  </si>
+  <si>
+    <t>getIndustryName()</t>
+  </si>
+  <si>
+    <t>Method to get the industry name</t>
+  </si>
+  <si>
+    <t>getProfession()</t>
+  </si>
+  <si>
+    <t>Method to get the profession name</t>
+  </si>
+  <si>
+    <t>DataGenerator.Country</t>
+  </si>
+  <si>
+    <t>getCountryName()</t>
+  </si>
+  <si>
+    <t>Method to get the country name</t>
+  </si>
+  <si>
+    <t>getCountryFlag()</t>
+  </si>
+  <si>
+    <t>Method to get the country flag as link</t>
+  </si>
+  <si>
+    <t>getCountryCurrency()</t>
+  </si>
+  <si>
+    <t>Method to get the country currency</t>
+  </si>
+  <si>
+    <t>getCountryCurrencyCode()</t>
+  </si>
+  <si>
+    <t>Method to get the country currency code</t>
+  </si>
+  <si>
+    <t>getCountryCapital()</t>
+  </si>
+  <si>
+    <t>Method to get the country capital</t>
+  </si>
+  <si>
+    <t>getCapitalCity()</t>
+  </si>
+  <si>
+    <t>Method to get the capital city</t>
+  </si>
+  <si>
+    <t>getLanguage()</t>
+  </si>
+  <si>
+    <t>Method to get the language</t>
+  </si>
+  <si>
+    <t>getNationality()</t>
+  </si>
+  <si>
+    <t>Method to get the nationality</t>
+  </si>
+  <si>
+    <t>DataGenerator.Demographic</t>
+  </si>
+  <si>
+    <t>getDemonym()</t>
+  </si>
+  <si>
+    <t>Method to get the demonym</t>
+  </si>
+  <si>
+    <t>getEducation()</t>
+  </si>
+  <si>
+    <t>Method to get the education attained</t>
+  </si>
+  <si>
+    <t>getMaritalStatus()</t>
+  </si>
+  <si>
+    <t>Method to get the marital status</t>
+  </si>
+  <si>
+    <t>getGender()</t>
+  </si>
+  <si>
+    <t>Method to get the gender</t>
+  </si>
+  <si>
+    <t>getRaceOrEthnicity()</t>
+  </si>
+  <si>
+    <t>Method to get the race or ethnicity</t>
+  </si>
+  <si>
+    <t>DataGenerator.Device</t>
+  </si>
+  <si>
+    <t>getPlatform()</t>
+  </si>
+  <si>
+    <t>Method to get the platform</t>
+  </si>
+  <si>
+    <t>getManufacturer()</t>
+  </si>
+  <si>
+    <t>Method to get the manufacturer</t>
+  </si>
+  <si>
+    <t>getModelName()</t>
+  </si>
+  <si>
+    <t>Method to get the model name</t>
+  </si>
+  <si>
+    <t>getSerialNumber()</t>
+  </si>
+  <si>
+    <t>Method to get the serial number</t>
+  </si>
+  <si>
+    <t>DataGenerator.File</t>
+  </si>
+  <si>
+    <t>getFileName()</t>
+  </si>
+  <si>
+    <t>Method to get the file name</t>
+  </si>
+  <si>
+    <t>getFileExtension()</t>
+  </si>
+  <si>
+    <t>Method to get the file extension</t>
+  </si>
+  <si>
+    <t>getMimeType()</t>
+  </si>
+  <si>
+    <t>Method to get the mime type</t>
+  </si>
+  <si>
+    <t>DataGenerator.Restaurant</t>
+  </si>
+  <si>
+    <t>getRestaurantName()</t>
+  </si>
+  <si>
+    <t>Method to get the restaurant name</t>
+  </si>
+  <si>
+    <t>getRestaurantType()</t>
+  </si>
+  <si>
+    <t>Method to get the restaurant type</t>
+  </si>
+  <si>
+    <t>getRestaurantReview()</t>
+  </si>
+  <si>
+    <t>Method to get the restaurant review</t>
+  </si>
+  <si>
+    <t>getRestaurantDescription()</t>
+  </si>
+  <si>
+    <t>Method to get the restaurant description</t>
+  </si>
+  <si>
+    <t>DataGenerator.Food</t>
+  </si>
+  <si>
+    <t>getDishName()</t>
+  </si>
+  <si>
+    <t>Method to get the dish name</t>
+  </si>
+  <si>
+    <t>getFruitName()</t>
+  </si>
+  <si>
+    <t>Method to get the fruit name</t>
+  </si>
+  <si>
+    <t>getIngredientName()</t>
+  </si>
+  <si>
+    <t>Method to get the ingredient name</t>
+  </si>
+  <si>
+    <t>getVegetableName()</t>
+  </si>
+  <si>
+    <t>Method to get the vegetable name</t>
+  </si>
+  <si>
+    <t>DataGenerator.Hobby</t>
+  </si>
+  <si>
+    <t>getActivityName()</t>
+  </si>
+  <si>
+    <t>Method to get the activity name</t>
+  </si>
+  <si>
+    <t>DataGenerator.Internet</t>
+  </si>
+  <si>
+    <t>getUserAgent()</t>
+  </si>
+  <si>
+    <t>Method to get the user agent</t>
+  </si>
+  <si>
+    <t>getDomainName()</t>
+  </si>
+  <si>
+    <t>Method to get the domain name</t>
+  </si>
+  <si>
+    <t>getEmailAddress()</t>
+  </si>
+  <si>
+    <t>Method to get the email address</t>
+  </si>
+  <si>
+    <t>getHTTPMethod()</t>
+  </si>
+  <si>
+    <t>Method to get the HTTP method</t>
+  </si>
+  <si>
+    <t>getImageURL()</t>
+  </si>
+  <si>
+    <t>Method to get the image URL</t>
+  </si>
+  <si>
+    <t>getImageURL(int width, int height)</t>
+  </si>
+  <si>
+    <t>getURL()</t>
+  </si>
+  <si>
+    <t>Method to get the URL</t>
+  </si>
+  <si>
+    <t>getMACAddress()</t>
+  </si>
+  <si>
+    <t>Method to get the MAC Address</t>
+  </si>
+  <si>
+    <t>getUUID()</t>
+  </si>
+  <si>
+    <t>Method to get the UUID</t>
+  </si>
+  <si>
+    <t>getPort()</t>
+  </si>
+  <si>
+    <t>Method to get the port number</t>
+  </si>
+  <si>
+    <t>DataGenerator.Job</t>
+  </si>
+  <si>
+    <t>getJobTitle()</t>
+  </si>
+  <si>
+    <t>Method to get the job title</t>
+  </si>
+  <si>
+    <t>getJobField()</t>
+  </si>
+  <si>
+    <t>Method to get the job field</t>
+  </si>
+  <si>
+    <t>getKeySkills()</t>
+  </si>
+  <si>
+    <t>Method to get the key skills</t>
+  </si>
+  <si>
+    <t>getJobPosition()</t>
+  </si>
+  <si>
+    <t>Method to get the job position</t>
+  </si>
+  <si>
+    <t>DataGenerator.Measurement</t>
+  </si>
+  <si>
+    <t>getHeight()</t>
+  </si>
+  <si>
+    <t>Method to get the height measurement names</t>
+  </si>
+  <si>
+    <t>getWeight()</t>
+  </si>
+  <si>
+    <t>Method to get the weight measurement names</t>
+  </si>
+  <si>
+    <t>getLength()</t>
+  </si>
+  <si>
+    <t>Method to get the length measurement names</t>
+  </si>
+  <si>
+    <t>getVolume()</t>
+  </si>
+  <si>
+    <t>Method to get the volume measurement names</t>
+  </si>
+  <si>
+    <t>DataGenerator.Medical</t>
+  </si>
+  <si>
+    <t>getHospitalName()</t>
+  </si>
+  <si>
+    <t>Method to get the hospital name</t>
+  </si>
+  <si>
+    <t>getDiseaseName()</t>
+  </si>
+  <si>
+    <t>Method to get the disease name</t>
+  </si>
+  <si>
+    <t>getMedicineName()</t>
+  </si>
+  <si>
+    <t>Method to get the medicine name</t>
+  </si>
+  <si>
+    <t>getDiagnosisCode()</t>
+  </si>
+  <si>
+    <t>Method to get the diagnosis code</t>
+  </si>
+  <si>
+    <t>getSymptoms()</t>
+  </si>
+  <si>
+    <t>Method to get the symptoms name</t>
+  </si>
+  <si>
+    <t>DataGenerator.Mountain</t>
+  </si>
+  <si>
+    <t>getMountainName()</t>
+  </si>
+  <si>
+    <t>Method to get the mountain name</t>
+  </si>
+  <si>
+    <t>getMountainRange()</t>
+  </si>
+  <si>
+    <t>Method to get the mountain range</t>
+  </si>
+  <si>
+    <t>DataGenerator.Number</t>
+  </si>
+  <si>
+    <t>getDigit()</t>
+  </si>
+  <si>
+    <t>Method to get the digit</t>
+  </si>
+  <si>
+    <t>getDigits(int count)</t>
+  </si>
+  <si>
+    <t>Method to get the digits based on count</t>
+  </si>
+  <si>
+    <t>getDigits(int min, int max)</t>
+  </si>
+  <si>
+    <t>Method to get the digits between minimum and maximum</t>
+  </si>
+  <si>
+    <t>getRandomDouble(int maxNumberOfDecimals, int min, int max)</t>
+  </si>
+  <si>
+    <t>Method to get the random double number</t>
+  </si>
+  <si>
+    <t>getNegativeNumber()</t>
+  </si>
+  <si>
+    <t>Method to get the negative number</t>
+  </si>
+  <si>
+    <t>DataGenerator.Vehicle</t>
+  </si>
+  <si>
+    <t>getVehicleManufacturer()</t>
+  </si>
+  <si>
+    <t>Method to get the vehicle manufacturer</t>
+  </si>
+  <si>
+    <t>getVehicleModel()</t>
+  </si>
+  <si>
+    <t>Method to get the vehicle model</t>
+  </si>
+  <si>
+    <t>getVehicleMake()</t>
+  </si>
+  <si>
+    <t>Method to get the vehicle make</t>
+  </si>
+  <si>
+    <t>getMakeAndModel()</t>
+  </si>
+  <si>
+    <t>Method to get the vehicle make and model</t>
+  </si>
+  <si>
+    <t>getFuelType()</t>
+  </si>
+  <si>
+    <t>Method to get the vehicle fuel type</t>
+  </si>
+  <si>
+    <t>getVehicleEngine()</t>
+  </si>
+  <si>
+    <t>Method to get the vehicle engine</t>
+  </si>
+  <si>
+    <t>getVehicleVIN()</t>
+  </si>
+  <si>
+    <t>Method to get the vehicle VIN</t>
+  </si>
+  <si>
+    <t>getVehicleLicensePlate()</t>
+  </si>
+  <si>
+    <t>Method to get the vehicle license plate</t>
+  </si>
+  <si>
+    <t>DataGenerator.Weather</t>
+  </si>
+  <si>
+    <t>getWeatherDescription()</t>
+  </si>
+  <si>
+    <t>Method to get the weather description</t>
+  </si>
+  <si>
+    <t>getTemperatureCelsius()</t>
+  </si>
+  <si>
+    <t>Method to get the temperature Celsius</t>
+  </si>
+  <si>
+    <t>getTemperatureCelsius(int minTemperature, int maxTemperature)</t>
+  </si>
+  <si>
+    <t>Method to get the temperature Celsius based on the minimum and maximum temperature</t>
+  </si>
+  <si>
+    <t>getTemperatureFahrenheit()</t>
+  </si>
+  <si>
+    <t>Method to get the temperature Fahrenheit</t>
+  </si>
+  <si>
+    <t>getTemperatureFahrenheit(int minTemperature, int maxTemperature)</t>
+  </si>
+  <si>
+    <t>Method to get the temperature Fahrenheit based on the minimum and maximum temperature</t>
+  </si>
+  <si>
+    <t>verifyFileDownloaded(String downloadPath, String fileName, String messageOnFailure)</t>
+  </si>
+  <si>
+    <t>Perform HTTP Post request with direct body data.</t>
+  </si>
+  <si>
+    <t>postRequestWithBody(String baseURI, String endPointPath, String requestBody, String authenticationScheme, String token, String contentType)</t>
+  </si>
+  <si>
+    <t>Perform HTTP Post request with direct body data with token</t>
+  </si>
+  <si>
+    <t>Perform HTTP Post request with body data from file.</t>
+  </si>
+  <si>
+    <t>postRequestWithGraphQL(String baseURI, String endPointPath, String graphQLQuery, String contentType)</t>
+  </si>
+  <si>
+    <t>Perform HTTP Post request with direct GraphQL data</t>
+  </si>
+  <si>
+    <t>postRequestWithGraphQLFile(String baseURI, String endPointPath, String graphQLQueryFileName, String contentType)</t>
+  </si>
+  <si>
+    <t>Perform HTTP Post request with GraphQL data from the file. The query text file should be placed in the GraphQL folder inside src/test/resources</t>
+  </si>
+  <si>
+    <t>postRequestWithGraphQLWithVariable(String baseURI, String endPointPath, String graphQLQuery, String variable, String contentType)</t>
+  </si>
+  <si>
+    <t>Perform HTTP Post request with direct GraphQL data and variables</t>
+  </si>
+  <si>
+    <t>postRequestWithGraphQLFilePath(String baseURI, String endPointPath, String graphQLQueryFilePath, String contentType)</t>
+  </si>
+  <si>
+    <t>Perform HTTP Post request with GraphQL data from the given file path. The file format should be in .txt</t>
+  </si>
+  <si>
+    <t>getRequestWithAuthToken(String baseURI, String endPointPath, String token, String pathParamName, String pathParamValue)</t>
+  </si>
+  <si>
+    <t>Perform HTTP Patch request with direct body data with token</t>
   </si>
 </sst>
 </file>
@@ -1737,13 +2809,13 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1887,6 +2959,67 @@
 </file>
 
 <file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Left Arrow 1">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12030075" y="19050"/>
+          <a:ext cx="409575" cy="171450"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-IN" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2722,10 +3855,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:D15"/>
+  <dimension ref="C2:D16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2736,10 +3869,10 @@
   <sheetData>
     <row r="2" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="3:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="37"/>
+      <c r="D3" s="38"/>
     </row>
     <row r="4" spans="3:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="21" t="s">
@@ -2778,7 +3911,7 @@
         <v>90</v>
       </c>
       <c r="D8" s="23">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="3:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -2823,19 +3956,27 @@
     </row>
     <row r="14" spans="3:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="21" t="s">
+        <v>414</v>
+      </c>
+      <c r="D14" s="23">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="15" spans="3:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="23">
+      <c r="D15" s="23">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="22" t="s">
+    <row r="16" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C16" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="20">
-        <f>SUM(D4:D14)</f>
-        <v>203</v>
+      <c r="D16" s="20">
+        <f>SUM(D4:D15)</f>
+        <v>367</v>
       </c>
     </row>
   </sheetData>
@@ -2850,10 +3991,11 @@
     <hyperlink ref="C11" location="AutomationEngine!A1" display="AutomationEngine"/>
     <hyperlink ref="C12" location="DataHandler!A1" display="DataHandler"/>
     <hyperlink ref="C13" location="DatabaseActions!A1" display="DatabaseActions"/>
-    <hyperlink ref="C14" location="AutomationReport!A1" display="AutomationReport"/>
+    <hyperlink ref="C15" location="AutomationReport!A1" display="AutomationReport"/>
     <hyperlink ref="C8" location="APIActions!A1" display="APIActions"/>
     <hyperlink ref="C9" location="APIValidations!A1" display="APIValidations"/>
     <hyperlink ref="C10" location="APIUtilities!A1" display="APIUtilities"/>
+    <hyperlink ref="C14" location="DataGenerator!A1" display="DataGenerator"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3204,6 +4346,2270 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D160"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="3" max="3" width="93.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="56.42578125" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="31">
+        <v>1</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>415</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>416</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="31">
+        <v>2</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>415</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>418</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="31">
+        <v>3</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>415</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>420</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="31">
+        <v>4</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>415</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>422</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="31">
+        <v>5</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>415</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>424</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="31">
+        <v>6</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>415</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>426</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="31">
+        <v>7</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>415</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>428</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="31">
+        <v>8</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>415</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>430</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="31">
+        <v>9</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>415</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>432</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="31">
+        <v>10</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>415</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>434</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="31">
+        <v>11</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>436</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>437</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="31">
+        <v>12</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>436</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>439</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="31">
+        <v>13</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>436</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>441</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="31">
+        <v>14</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>436</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>443</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="31">
+        <v>15</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>436</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>445</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="31">
+        <v>16</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>436</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>447</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="31">
+        <v>17</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>436</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>449</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="31">
+        <v>18</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>436</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>451</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="31">
+        <v>19</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>436</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>453</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="31">
+        <v>20</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>436</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>455</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="31">
+        <v>21</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>436</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>457</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="31">
+        <v>22</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>436</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>459</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="31">
+        <v>23</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>436</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>461</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="31">
+        <v>24</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>436</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>463</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="31">
+        <v>25</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>436</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>465</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="31">
+        <v>26</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>436</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>467</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="31">
+        <v>27</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>436</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>469</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="31">
+        <v>28</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>436</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>471</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="31">
+        <v>29</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>436</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>473</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="31">
+        <v>30</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>436</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>475</v>
+      </c>
+      <c r="D31" s="15" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="31">
+        <v>31</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>436</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>477</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="31">
+        <v>32</v>
+      </c>
+      <c r="B33" s="16" t="s">
+        <v>436</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>479</v>
+      </c>
+      <c r="D33" s="15" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="31">
+        <v>33</v>
+      </c>
+      <c r="B34" s="16" t="s">
+        <v>436</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>481</v>
+      </c>
+      <c r="D34" s="15" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="31">
+        <v>34</v>
+      </c>
+      <c r="B35" s="16" t="s">
+        <v>436</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>483</v>
+      </c>
+      <c r="D35" s="15" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="31">
+        <v>35</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>436</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>485</v>
+      </c>
+      <c r="D36" s="15" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="31">
+        <v>36</v>
+      </c>
+      <c r="B37" s="16" t="s">
+        <v>436</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>487</v>
+      </c>
+      <c r="D37" s="15" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="31">
+        <v>37</v>
+      </c>
+      <c r="B38" s="16" t="s">
+        <v>489</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>490</v>
+      </c>
+      <c r="D38" s="15" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="31">
+        <v>38</v>
+      </c>
+      <c r="B39" s="16" t="s">
+        <v>489</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>492</v>
+      </c>
+      <c r="D39" s="15" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="31">
+        <v>39</v>
+      </c>
+      <c r="B40" s="16" t="s">
+        <v>489</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>494</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="31">
+        <v>40</v>
+      </c>
+      <c r="B41" s="16" t="s">
+        <v>489</v>
+      </c>
+      <c r="C41" s="14" t="s">
+        <v>496</v>
+      </c>
+      <c r="D41" s="15" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="31">
+        <v>41</v>
+      </c>
+      <c r="B42" s="16" t="s">
+        <v>498</v>
+      </c>
+      <c r="C42" s="14" t="s">
+        <v>499</v>
+      </c>
+      <c r="D42" s="15" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="31">
+        <v>42</v>
+      </c>
+      <c r="B43" s="16" t="s">
+        <v>498</v>
+      </c>
+      <c r="C43" s="14" t="s">
+        <v>501</v>
+      </c>
+      <c r="D43" s="15" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="31">
+        <v>43</v>
+      </c>
+      <c r="B44" s="16" t="s">
+        <v>498</v>
+      </c>
+      <c r="C44" s="14" t="s">
+        <v>503</v>
+      </c>
+      <c r="D44" s="15" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="31">
+        <v>44</v>
+      </c>
+      <c r="B45" s="16" t="s">
+        <v>498</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>505</v>
+      </c>
+      <c r="D45" s="15" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="31">
+        <v>45</v>
+      </c>
+      <c r="B46" s="16" t="s">
+        <v>507</v>
+      </c>
+      <c r="C46" s="14" t="s">
+        <v>508</v>
+      </c>
+      <c r="D46" s="15" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="31">
+        <v>46</v>
+      </c>
+      <c r="B47" s="16" t="s">
+        <v>507</v>
+      </c>
+      <c r="C47" s="14" t="s">
+        <v>510</v>
+      </c>
+      <c r="D47" s="15" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="31">
+        <v>47</v>
+      </c>
+      <c r="B48" s="16" t="s">
+        <v>512</v>
+      </c>
+      <c r="C48" s="14" t="s">
+        <v>513</v>
+      </c>
+      <c r="D48" s="15" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="31">
+        <v>48</v>
+      </c>
+      <c r="B49" s="16" t="s">
+        <v>515</v>
+      </c>
+      <c r="C49" s="14" t="s">
+        <v>516</v>
+      </c>
+      <c r="D49" s="15" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="31">
+        <v>49</v>
+      </c>
+      <c r="B50" s="16" t="s">
+        <v>515</v>
+      </c>
+      <c r="C50" s="14" t="s">
+        <v>518</v>
+      </c>
+      <c r="D50" s="15" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="31">
+        <v>50</v>
+      </c>
+      <c r="B51" s="16" t="s">
+        <v>515</v>
+      </c>
+      <c r="C51" s="14" t="s">
+        <v>520</v>
+      </c>
+      <c r="D51" s="15" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="31">
+        <v>51</v>
+      </c>
+      <c r="B52" s="16" t="s">
+        <v>515</v>
+      </c>
+      <c r="C52" s="14" t="s">
+        <v>522</v>
+      </c>
+      <c r="D52" s="15" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="31">
+        <v>52</v>
+      </c>
+      <c r="B53" s="16" t="s">
+        <v>515</v>
+      </c>
+      <c r="C53" s="14" t="s">
+        <v>524</v>
+      </c>
+      <c r="D53" s="15" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="31">
+        <v>53</v>
+      </c>
+      <c r="B54" s="16" t="s">
+        <v>515</v>
+      </c>
+      <c r="C54" s="14" t="s">
+        <v>526</v>
+      </c>
+      <c r="D54" s="15" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="31">
+        <v>54</v>
+      </c>
+      <c r="B55" s="16" t="s">
+        <v>515</v>
+      </c>
+      <c r="C55" s="14" t="s">
+        <v>528</v>
+      </c>
+      <c r="D55" s="15" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="31">
+        <v>55</v>
+      </c>
+      <c r="B56" s="16" t="s">
+        <v>515</v>
+      </c>
+      <c r="C56" s="14" t="s">
+        <v>530</v>
+      </c>
+      <c r="D56" s="15" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="31">
+        <v>56</v>
+      </c>
+      <c r="B57" s="16" t="s">
+        <v>532</v>
+      </c>
+      <c r="C57" s="14" t="s">
+        <v>533</v>
+      </c>
+      <c r="D57" s="15" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" s="31">
+        <v>57</v>
+      </c>
+      <c r="B58" s="16" t="s">
+        <v>532</v>
+      </c>
+      <c r="C58" s="14" t="s">
+        <v>535</v>
+      </c>
+      <c r="D58" s="15" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="31">
+        <v>58</v>
+      </c>
+      <c r="B59" s="16" t="s">
+        <v>537</v>
+      </c>
+      <c r="C59" s="14" t="s">
+        <v>538</v>
+      </c>
+      <c r="D59" s="15" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="31">
+        <v>59</v>
+      </c>
+      <c r="B60" s="16" t="s">
+        <v>537</v>
+      </c>
+      <c r="C60" s="14" t="s">
+        <v>540</v>
+      </c>
+      <c r="D60" s="15" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="31">
+        <v>60</v>
+      </c>
+      <c r="B61" s="16" t="s">
+        <v>537</v>
+      </c>
+      <c r="C61" s="14" t="s">
+        <v>542</v>
+      </c>
+      <c r="D61" s="15" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="31">
+        <v>61</v>
+      </c>
+      <c r="B62" s="16" t="s">
+        <v>537</v>
+      </c>
+      <c r="C62" s="14" t="s">
+        <v>544</v>
+      </c>
+      <c r="D62" s="15" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="31">
+        <v>62</v>
+      </c>
+      <c r="B63" s="16" t="s">
+        <v>537</v>
+      </c>
+      <c r="C63" s="14" t="s">
+        <v>546</v>
+      </c>
+      <c r="D63" s="15" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="31">
+        <v>63</v>
+      </c>
+      <c r="B64" s="16" t="s">
+        <v>537</v>
+      </c>
+      <c r="C64" s="14" t="s">
+        <v>548</v>
+      </c>
+      <c r="D64" s="15" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="31">
+        <v>64</v>
+      </c>
+      <c r="B65" s="16" t="s">
+        <v>537</v>
+      </c>
+      <c r="C65" s="14" t="s">
+        <v>550</v>
+      </c>
+      <c r="D65" s="15" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="31">
+        <v>65</v>
+      </c>
+      <c r="B66" s="16" t="s">
+        <v>552</v>
+      </c>
+      <c r="C66" s="14" t="s">
+        <v>553</v>
+      </c>
+      <c r="D66" s="15" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="31">
+        <v>66</v>
+      </c>
+      <c r="B67" s="16" t="s">
+        <v>552</v>
+      </c>
+      <c r="C67" s="14" t="s">
+        <v>555</v>
+      </c>
+      <c r="D67" s="15" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="31">
+        <v>67</v>
+      </c>
+      <c r="B68" s="16" t="s">
+        <v>552</v>
+      </c>
+      <c r="C68" s="14" t="s">
+        <v>557</v>
+      </c>
+      <c r="D68" s="15" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="31">
+        <v>68</v>
+      </c>
+      <c r="B69" s="16" t="s">
+        <v>552</v>
+      </c>
+      <c r="C69" s="14" t="s">
+        <v>559</v>
+      </c>
+      <c r="D69" s="15" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="31">
+        <v>69</v>
+      </c>
+      <c r="B70" s="16" t="s">
+        <v>552</v>
+      </c>
+      <c r="C70" s="14" t="s">
+        <v>561</v>
+      </c>
+      <c r="D70" s="15" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="31">
+        <v>70</v>
+      </c>
+      <c r="B71" s="16" t="s">
+        <v>563</v>
+      </c>
+      <c r="C71" s="14" t="s">
+        <v>564</v>
+      </c>
+      <c r="D71" s="15" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="31">
+        <v>71</v>
+      </c>
+      <c r="B72" s="16" t="s">
+        <v>563</v>
+      </c>
+      <c r="C72" s="14" t="s">
+        <v>566</v>
+      </c>
+      <c r="D72" s="15" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="31">
+        <v>72</v>
+      </c>
+      <c r="B73" s="16" t="s">
+        <v>563</v>
+      </c>
+      <c r="C73" s="14" t="s">
+        <v>568</v>
+      </c>
+      <c r="D73" s="15" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="31">
+        <v>73</v>
+      </c>
+      <c r="B74" s="16" t="s">
+        <v>563</v>
+      </c>
+      <c r="C74" s="14" t="s">
+        <v>570</v>
+      </c>
+      <c r="D74" s="15" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="31">
+        <v>74</v>
+      </c>
+      <c r="B75" s="16" t="s">
+        <v>563</v>
+      </c>
+      <c r="C75" s="14" t="s">
+        <v>572</v>
+      </c>
+      <c r="D75" s="15" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="31">
+        <v>75</v>
+      </c>
+      <c r="B76" s="16" t="s">
+        <v>563</v>
+      </c>
+      <c r="C76" s="14" t="s">
+        <v>574</v>
+      </c>
+      <c r="D76" s="15" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="31">
+        <v>76</v>
+      </c>
+      <c r="B77" s="16" t="s">
+        <v>576</v>
+      </c>
+      <c r="C77" s="14" t="s">
+        <v>577</v>
+      </c>
+      <c r="D77" s="15" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="31">
+        <v>77</v>
+      </c>
+      <c r="B78" s="16" t="s">
+        <v>576</v>
+      </c>
+      <c r="C78" s="14" t="s">
+        <v>579</v>
+      </c>
+      <c r="D78" s="15" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A79" s="31">
+        <v>78</v>
+      </c>
+      <c r="B79" s="16" t="s">
+        <v>576</v>
+      </c>
+      <c r="C79" s="14" t="s">
+        <v>581</v>
+      </c>
+      <c r="D79" s="15" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="31">
+        <v>79</v>
+      </c>
+      <c r="B80" s="16" t="s">
+        <v>583</v>
+      </c>
+      <c r="C80" s="14" t="s">
+        <v>584</v>
+      </c>
+      <c r="D80" s="15" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="31">
+        <v>80</v>
+      </c>
+      <c r="B81" s="16" t="s">
+        <v>583</v>
+      </c>
+      <c r="C81" s="14" t="s">
+        <v>586</v>
+      </c>
+      <c r="D81" s="15" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="31">
+        <v>81</v>
+      </c>
+      <c r="B82" s="16" t="s">
+        <v>583</v>
+      </c>
+      <c r="C82" s="14" t="s">
+        <v>588</v>
+      </c>
+      <c r="D82" s="15" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="31">
+        <v>82</v>
+      </c>
+      <c r="B83" s="16" t="s">
+        <v>583</v>
+      </c>
+      <c r="C83" s="14" t="s">
+        <v>590</v>
+      </c>
+      <c r="D83" s="15" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="31">
+        <v>83</v>
+      </c>
+      <c r="B84" s="16" t="s">
+        <v>592</v>
+      </c>
+      <c r="C84" s="14" t="s">
+        <v>593</v>
+      </c>
+      <c r="D84" s="15" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="31">
+        <v>84</v>
+      </c>
+      <c r="B85" s="16" t="s">
+        <v>592</v>
+      </c>
+      <c r="C85" s="14" t="s">
+        <v>595</v>
+      </c>
+      <c r="D85" s="15" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="31">
+        <v>85</v>
+      </c>
+      <c r="B86" s="16" t="s">
+        <v>592</v>
+      </c>
+      <c r="C86" s="14" t="s">
+        <v>597</v>
+      </c>
+      <c r="D86" s="15" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="31">
+        <v>86</v>
+      </c>
+      <c r="B87" s="16" t="s">
+        <v>592</v>
+      </c>
+      <c r="C87" s="14" t="s">
+        <v>599</v>
+      </c>
+      <c r="D87" s="15" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="31">
+        <v>87</v>
+      </c>
+      <c r="B88" s="16" t="s">
+        <v>592</v>
+      </c>
+      <c r="C88" s="14" t="s">
+        <v>601</v>
+      </c>
+      <c r="D88" s="15" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="31">
+        <v>88</v>
+      </c>
+      <c r="B89" s="16" t="s">
+        <v>603</v>
+      </c>
+      <c r="C89" s="14" t="s">
+        <v>604</v>
+      </c>
+      <c r="D89" s="15" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="31">
+        <v>89</v>
+      </c>
+      <c r="B90" s="16" t="s">
+        <v>603</v>
+      </c>
+      <c r="C90" s="14" t="s">
+        <v>606</v>
+      </c>
+      <c r="D90" s="15" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="31">
+        <v>90</v>
+      </c>
+      <c r="B91" s="16" t="s">
+        <v>603</v>
+      </c>
+      <c r="C91" s="14" t="s">
+        <v>608</v>
+      </c>
+      <c r="D91" s="15" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="31">
+        <v>91</v>
+      </c>
+      <c r="B92" s="16" t="s">
+        <v>603</v>
+      </c>
+      <c r="C92" s="14" t="s">
+        <v>610</v>
+      </c>
+      <c r="D92" s="15" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="31">
+        <v>92</v>
+      </c>
+      <c r="B93" s="16" t="s">
+        <v>603</v>
+      </c>
+      <c r="C93" s="14" t="s">
+        <v>612</v>
+      </c>
+      <c r="D93" s="15" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="31">
+        <v>93</v>
+      </c>
+      <c r="B94" s="16" t="s">
+        <v>603</v>
+      </c>
+      <c r="C94" s="14" t="s">
+        <v>614</v>
+      </c>
+      <c r="D94" s="15" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="31">
+        <v>94</v>
+      </c>
+      <c r="B95" s="16" t="s">
+        <v>603</v>
+      </c>
+      <c r="C95" s="14" t="s">
+        <v>616</v>
+      </c>
+      <c r="D95" s="15" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="31">
+        <v>95</v>
+      </c>
+      <c r="B96" s="16" t="s">
+        <v>603</v>
+      </c>
+      <c r="C96" s="14" t="s">
+        <v>618</v>
+      </c>
+      <c r="D96" s="15" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="31">
+        <v>96</v>
+      </c>
+      <c r="B97" s="16" t="s">
+        <v>620</v>
+      </c>
+      <c r="C97" s="14" t="s">
+        <v>621</v>
+      </c>
+      <c r="D97" s="15" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="31">
+        <v>97</v>
+      </c>
+      <c r="B98" s="16" t="s">
+        <v>620</v>
+      </c>
+      <c r="C98" s="14" t="s">
+        <v>623</v>
+      </c>
+      <c r="D98" s="15" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="31">
+        <v>98</v>
+      </c>
+      <c r="B99" s="16" t="s">
+        <v>620</v>
+      </c>
+      <c r="C99" s="14" t="s">
+        <v>625</v>
+      </c>
+      <c r="D99" s="15" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="31">
+        <v>99</v>
+      </c>
+      <c r="B100" s="16" t="s">
+        <v>620</v>
+      </c>
+      <c r="C100" s="14" t="s">
+        <v>627</v>
+      </c>
+      <c r="D100" s="15" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="31">
+        <v>100</v>
+      </c>
+      <c r="B101" s="16" t="s">
+        <v>620</v>
+      </c>
+      <c r="C101" s="14" t="s">
+        <v>629</v>
+      </c>
+      <c r="D101" s="15" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="31">
+        <v>101</v>
+      </c>
+      <c r="B102" s="16" t="s">
+        <v>631</v>
+      </c>
+      <c r="C102" s="14" t="s">
+        <v>632</v>
+      </c>
+      <c r="D102" s="15" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="31">
+        <v>102</v>
+      </c>
+      <c r="B103" s="16" t="s">
+        <v>631</v>
+      </c>
+      <c r="C103" s="14" t="s">
+        <v>634</v>
+      </c>
+      <c r="D103" s="15" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="31">
+        <v>103</v>
+      </c>
+      <c r="B104" s="16" t="s">
+        <v>631</v>
+      </c>
+      <c r="C104" s="14" t="s">
+        <v>636</v>
+      </c>
+      <c r="D104" s="15" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="31">
+        <v>104</v>
+      </c>
+      <c r="B105" s="16" t="s">
+        <v>631</v>
+      </c>
+      <c r="C105" s="14" t="s">
+        <v>638</v>
+      </c>
+      <c r="D105" s="15" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="31">
+        <v>105</v>
+      </c>
+      <c r="B106" s="16" t="s">
+        <v>640</v>
+      </c>
+      <c r="C106" s="14" t="s">
+        <v>641</v>
+      </c>
+      <c r="D106" s="15" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="31">
+        <v>106</v>
+      </c>
+      <c r="B107" s="16" t="s">
+        <v>640</v>
+      </c>
+      <c r="C107" s="14" t="s">
+        <v>643</v>
+      </c>
+      <c r="D107" s="15" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="31">
+        <v>107</v>
+      </c>
+      <c r="B108" s="16" t="s">
+        <v>640</v>
+      </c>
+      <c r="C108" s="14" t="s">
+        <v>645</v>
+      </c>
+      <c r="D108" s="15" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="31">
+        <v>108</v>
+      </c>
+      <c r="B109" s="16" t="s">
+        <v>647</v>
+      </c>
+      <c r="C109" s="14" t="s">
+        <v>648</v>
+      </c>
+      <c r="D109" s="15" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" s="31">
+        <v>109</v>
+      </c>
+      <c r="B110" s="16" t="s">
+        <v>647</v>
+      </c>
+      <c r="C110" s="14" t="s">
+        <v>650</v>
+      </c>
+      <c r="D110" s="15" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" s="31">
+        <v>110</v>
+      </c>
+      <c r="B111" s="16" t="s">
+        <v>647</v>
+      </c>
+      <c r="C111" s="14" t="s">
+        <v>652</v>
+      </c>
+      <c r="D111" s="15" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="31">
+        <v>111</v>
+      </c>
+      <c r="B112" s="16" t="s">
+        <v>647</v>
+      </c>
+      <c r="C112" s="14" t="s">
+        <v>654</v>
+      </c>
+      <c r="D112" s="15" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" s="31">
+        <v>112</v>
+      </c>
+      <c r="B113" s="16" t="s">
+        <v>656</v>
+      </c>
+      <c r="C113" s="14" t="s">
+        <v>657</v>
+      </c>
+      <c r="D113" s="15" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" s="31">
+        <v>113</v>
+      </c>
+      <c r="B114" s="16" t="s">
+        <v>656</v>
+      </c>
+      <c r="C114" s="14" t="s">
+        <v>659</v>
+      </c>
+      <c r="D114" s="15" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" s="31">
+        <v>114</v>
+      </c>
+      <c r="B115" s="16" t="s">
+        <v>656</v>
+      </c>
+      <c r="C115" s="14" t="s">
+        <v>661</v>
+      </c>
+      <c r="D115" s="15" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" s="31">
+        <v>115</v>
+      </c>
+      <c r="B116" s="16" t="s">
+        <v>656</v>
+      </c>
+      <c r="C116" s="14" t="s">
+        <v>663</v>
+      </c>
+      <c r="D116" s="15" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" s="31">
+        <v>116</v>
+      </c>
+      <c r="B117" s="16" t="s">
+        <v>665</v>
+      </c>
+      <c r="C117" s="14" t="s">
+        <v>666</v>
+      </c>
+      <c r="D117" s="15" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" s="31">
+        <v>117</v>
+      </c>
+      <c r="B118" s="16" t="s">
+        <v>668</v>
+      </c>
+      <c r="C118" s="14" t="s">
+        <v>669</v>
+      </c>
+      <c r="D118" s="15" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" s="31">
+        <v>118</v>
+      </c>
+      <c r="B119" s="16" t="s">
+        <v>668</v>
+      </c>
+      <c r="C119" s="14" t="s">
+        <v>671</v>
+      </c>
+      <c r="D119" s="15" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" s="31">
+        <v>119</v>
+      </c>
+      <c r="B120" s="16" t="s">
+        <v>668</v>
+      </c>
+      <c r="C120" s="14" t="s">
+        <v>673</v>
+      </c>
+      <c r="D120" s="15" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" s="31">
+        <v>120</v>
+      </c>
+      <c r="B121" s="16" t="s">
+        <v>668</v>
+      </c>
+      <c r="C121" s="14" t="s">
+        <v>675</v>
+      </c>
+      <c r="D121" s="15" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" s="31">
+        <v>121</v>
+      </c>
+      <c r="B122" s="16" t="s">
+        <v>668</v>
+      </c>
+      <c r="C122" s="14" t="s">
+        <v>677</v>
+      </c>
+      <c r="D122" s="15" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" s="31">
+        <v>122</v>
+      </c>
+      <c r="B123" s="16" t="s">
+        <v>668</v>
+      </c>
+      <c r="C123" s="14" t="s">
+        <v>679</v>
+      </c>
+      <c r="D123" s="15" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" s="31">
+        <v>123</v>
+      </c>
+      <c r="B124" s="16" t="s">
+        <v>668</v>
+      </c>
+      <c r="C124" s="14" t="s">
+        <v>680</v>
+      </c>
+      <c r="D124" s="15" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" s="31">
+        <v>124</v>
+      </c>
+      <c r="B125" s="16" t="s">
+        <v>668</v>
+      </c>
+      <c r="C125" s="14" t="s">
+        <v>682</v>
+      </c>
+      <c r="D125" s="15" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" s="31">
+        <v>125</v>
+      </c>
+      <c r="B126" s="16" t="s">
+        <v>668</v>
+      </c>
+      <c r="C126" s="14" t="s">
+        <v>684</v>
+      </c>
+      <c r="D126" s="15" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" s="31">
+        <v>126</v>
+      </c>
+      <c r="B127" s="16" t="s">
+        <v>668</v>
+      </c>
+      <c r="C127" s="14" t="s">
+        <v>686</v>
+      </c>
+      <c r="D127" s="15" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" s="31">
+        <v>127</v>
+      </c>
+      <c r="B128" s="16" t="s">
+        <v>688</v>
+      </c>
+      <c r="C128" s="14" t="s">
+        <v>689</v>
+      </c>
+      <c r="D128" s="15" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" s="31">
+        <v>128</v>
+      </c>
+      <c r="B129" s="16" t="s">
+        <v>688</v>
+      </c>
+      <c r="C129" s="14" t="s">
+        <v>691</v>
+      </c>
+      <c r="D129" s="15" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" s="31">
+        <v>129</v>
+      </c>
+      <c r="B130" s="16" t="s">
+        <v>688</v>
+      </c>
+      <c r="C130" s="14" t="s">
+        <v>693</v>
+      </c>
+      <c r="D130" s="15" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" s="31">
+        <v>130</v>
+      </c>
+      <c r="B131" s="16" t="s">
+        <v>688</v>
+      </c>
+      <c r="C131" s="14" t="s">
+        <v>695</v>
+      </c>
+      <c r="D131" s="15" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" s="31">
+        <v>131</v>
+      </c>
+      <c r="B132" s="16" t="s">
+        <v>697</v>
+      </c>
+      <c r="C132" s="14" t="s">
+        <v>698</v>
+      </c>
+      <c r="D132" s="15" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" s="31">
+        <v>132</v>
+      </c>
+      <c r="B133" s="16" t="s">
+        <v>697</v>
+      </c>
+      <c r="C133" s="14" t="s">
+        <v>700</v>
+      </c>
+      <c r="D133" s="15" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" s="31">
+        <v>133</v>
+      </c>
+      <c r="B134" s="16" t="s">
+        <v>697</v>
+      </c>
+      <c r="C134" s="14" t="s">
+        <v>702</v>
+      </c>
+      <c r="D134" s="15" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" s="31">
+        <v>134</v>
+      </c>
+      <c r="B135" s="16" t="s">
+        <v>697</v>
+      </c>
+      <c r="C135" s="14" t="s">
+        <v>704</v>
+      </c>
+      <c r="D135" s="15" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" s="31">
+        <v>135</v>
+      </c>
+      <c r="B136" s="16" t="s">
+        <v>706</v>
+      </c>
+      <c r="C136" s="14" t="s">
+        <v>707</v>
+      </c>
+      <c r="D136" s="15" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" s="31">
+        <v>136</v>
+      </c>
+      <c r="B137" s="16" t="s">
+        <v>706</v>
+      </c>
+      <c r="C137" s="14" t="s">
+        <v>709</v>
+      </c>
+      <c r="D137" s="15" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" s="31">
+        <v>137</v>
+      </c>
+      <c r="B138" s="16" t="s">
+        <v>706</v>
+      </c>
+      <c r="C138" s="14" t="s">
+        <v>711</v>
+      </c>
+      <c r="D138" s="15" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139" s="31">
+        <v>138</v>
+      </c>
+      <c r="B139" s="16" t="s">
+        <v>706</v>
+      </c>
+      <c r="C139" s="14" t="s">
+        <v>713</v>
+      </c>
+      <c r="D139" s="15" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" s="31">
+        <v>139</v>
+      </c>
+      <c r="B140" s="16" t="s">
+        <v>706</v>
+      </c>
+      <c r="C140" s="14" t="s">
+        <v>715</v>
+      </c>
+      <c r="D140" s="15" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141" s="31">
+        <v>140</v>
+      </c>
+      <c r="B141" s="16" t="s">
+        <v>717</v>
+      </c>
+      <c r="C141" s="14" t="s">
+        <v>718</v>
+      </c>
+      <c r="D141" s="15" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A142" s="31">
+        <v>141</v>
+      </c>
+      <c r="B142" s="16" t="s">
+        <v>717</v>
+      </c>
+      <c r="C142" s="14" t="s">
+        <v>720</v>
+      </c>
+      <c r="D142" s="15" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" s="31">
+        <v>142</v>
+      </c>
+      <c r="B143" s="16" t="s">
+        <v>722</v>
+      </c>
+      <c r="C143" s="14" t="s">
+        <v>723</v>
+      </c>
+      <c r="D143" s="15" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144" s="31">
+        <v>143</v>
+      </c>
+      <c r="B144" s="16" t="s">
+        <v>722</v>
+      </c>
+      <c r="C144" s="14" t="s">
+        <v>725</v>
+      </c>
+      <c r="D144" s="15" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145" s="31">
+        <v>144</v>
+      </c>
+      <c r="B145" s="16" t="s">
+        <v>722</v>
+      </c>
+      <c r="C145" s="14" t="s">
+        <v>727</v>
+      </c>
+      <c r="D145" s="15" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" s="31">
+        <v>145</v>
+      </c>
+      <c r="B146" s="16" t="s">
+        <v>722</v>
+      </c>
+      <c r="C146" s="14" t="s">
+        <v>729</v>
+      </c>
+      <c r="D146" s="15" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" s="31">
+        <v>146</v>
+      </c>
+      <c r="B147" s="16" t="s">
+        <v>722</v>
+      </c>
+      <c r="C147" s="14" t="s">
+        <v>731</v>
+      </c>
+      <c r="D147" s="15" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A148" s="31">
+        <v>147</v>
+      </c>
+      <c r="B148" s="16" t="s">
+        <v>733</v>
+      </c>
+      <c r="C148" s="14" t="s">
+        <v>734</v>
+      </c>
+      <c r="D148" s="15" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A149" s="31">
+        <v>148</v>
+      </c>
+      <c r="B149" s="16" t="s">
+        <v>733</v>
+      </c>
+      <c r="C149" s="14" t="s">
+        <v>736</v>
+      </c>
+      <c r="D149" s="15" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A150" s="31">
+        <v>149</v>
+      </c>
+      <c r="B150" s="16" t="s">
+        <v>733</v>
+      </c>
+      <c r="C150" s="14" t="s">
+        <v>738</v>
+      </c>
+      <c r="D150" s="15" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A151" s="31">
+        <v>150</v>
+      </c>
+      <c r="B151" s="16" t="s">
+        <v>733</v>
+      </c>
+      <c r="C151" s="14" t="s">
+        <v>740</v>
+      </c>
+      <c r="D151" s="15" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A152" s="31">
+        <v>151</v>
+      </c>
+      <c r="B152" s="16" t="s">
+        <v>733</v>
+      </c>
+      <c r="C152" s="14" t="s">
+        <v>742</v>
+      </c>
+      <c r="D152" s="15" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A153" s="31">
+        <v>152</v>
+      </c>
+      <c r="B153" s="16" t="s">
+        <v>733</v>
+      </c>
+      <c r="C153" s="14" t="s">
+        <v>744</v>
+      </c>
+      <c r="D153" s="15" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154" s="31">
+        <v>153</v>
+      </c>
+      <c r="B154" s="16" t="s">
+        <v>733</v>
+      </c>
+      <c r="C154" s="14" t="s">
+        <v>746</v>
+      </c>
+      <c r="D154" s="15" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A155" s="31">
+        <v>154</v>
+      </c>
+      <c r="B155" s="16" t="s">
+        <v>733</v>
+      </c>
+      <c r="C155" s="14" t="s">
+        <v>748</v>
+      </c>
+      <c r="D155" s="15" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A156" s="31">
+        <v>155</v>
+      </c>
+      <c r="B156" s="16" t="s">
+        <v>750</v>
+      </c>
+      <c r="C156" s="14" t="s">
+        <v>751</v>
+      </c>
+      <c r="D156" s="15" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157" s="31">
+        <v>156</v>
+      </c>
+      <c r="B157" s="16" t="s">
+        <v>750</v>
+      </c>
+      <c r="C157" s="14" t="s">
+        <v>753</v>
+      </c>
+      <c r="D157" s="15" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A158" s="31">
+        <v>157</v>
+      </c>
+      <c r="B158" s="16" t="s">
+        <v>750</v>
+      </c>
+      <c r="C158" s="14" t="s">
+        <v>755</v>
+      </c>
+      <c r="D158" s="15" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A159" s="31">
+        <v>158</v>
+      </c>
+      <c r="B159" s="16" t="s">
+        <v>750</v>
+      </c>
+      <c r="C159" s="14" t="s">
+        <v>757</v>
+      </c>
+      <c r="D159" s="15" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A160" s="32">
+        <v>159</v>
+      </c>
+      <c r="B160" s="26" t="s">
+        <v>750</v>
+      </c>
+      <c r="C160" s="17" t="s">
+        <v>759</v>
+      </c>
+      <c r="D160" s="18" t="s">
+        <v>760</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4498,7 +7904,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4769,10 +8175,10 @@
         <v>341</v>
       </c>
       <c r="C19" s="5" t="s">
+        <v>761</v>
+      </c>
+      <c r="D19" s="6" t="s">
         <v>374</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4783,7 +8189,7 @@
         <v>341</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>66</v>
@@ -4797,7 +8203,7 @@
         <v>341</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>67</v>
@@ -4811,7 +8217,7 @@
         <v>341</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>69</v>
@@ -4825,7 +8231,7 @@
         <v>341</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>68</v>
@@ -4839,7 +8245,7 @@
         <v>341</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>69</v>
@@ -4853,7 +8259,7 @@
         <v>341</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>131</v>
@@ -4867,7 +8273,7 @@
         <v>341</v>
       </c>
       <c r="C26" s="24" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D26" s="25" t="s">
         <v>132</v>
@@ -4919,7 +8325,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D2" s="15" t="s">
         <v>70</v>
@@ -4933,7 +8339,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D3" s="15" t="s">
         <v>82</v>
@@ -4947,7 +8353,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D4" s="15" t="s">
         <v>78</v>
@@ -4961,7 +8367,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D5" s="15" t="s">
         <v>77</v>
@@ -4975,7 +8381,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D6" s="15" t="s">
         <v>80</v>
@@ -4989,7 +8395,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D7" s="15" t="s">
         <v>81</v>
@@ -5003,7 +8409,7 @@
         <v>5</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D8" s="15" t="s">
         <v>71</v>
@@ -5017,7 +8423,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D9" s="15" t="s">
         <v>79</v>
@@ -5031,7 +8437,7 @@
         <v>5</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D10" s="15" t="s">
         <v>85</v>
@@ -5045,7 +8451,7 @@
         <v>5</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D11" s="15" t="s">
         <v>75</v>
@@ -5059,7 +8465,7 @@
         <v>5</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D12" s="15" t="s">
         <v>86</v>
@@ -5073,7 +8479,7 @@
         <v>5</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D13" s="15" t="s">
         <v>87</v>
@@ -5087,7 +8493,7 @@
         <v>5</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D14" s="15" t="s">
         <v>88</v>
@@ -5101,7 +8507,7 @@
         <v>5</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D15" s="15" t="s">
         <v>84</v>
@@ -5115,7 +8521,7 @@
         <v>5</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D16" s="15" t="s">
         <v>73</v>
@@ -5129,7 +8535,7 @@
         <v>5</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D17" s="15" t="s">
         <v>72</v>
@@ -5143,7 +8549,7 @@
         <v>5</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D18" s="15" t="s">
         <v>76</v>
@@ -5157,7 +8563,7 @@
         <v>5</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D19" s="15" t="s">
         <v>74</v>
@@ -5171,7 +8577,7 @@
         <v>5</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D20" s="15" t="s">
         <v>83</v>
@@ -5185,7 +8591,7 @@
         <v>5</v>
       </c>
       <c r="C21" s="26" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D21" s="18" t="s">
         <v>89</v>
@@ -5251,7 +8657,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>200</v>
@@ -5294,7 +8700,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -5324,240 +8730,310 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="38">
+      <c r="A2" s="36">
         <v>1</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="16" t="s">
         <v>90</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="15" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="38">
+      <c r="A3" s="36">
         <v>2</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="16" t="s">
         <v>90</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="15" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="38">
+      <c r="A4" s="36">
         <v>3</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="16" t="s">
         <v>90</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="15" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="38">
+      <c r="A5" s="36">
         <v>4</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="16" t="s">
         <v>90</v>
       </c>
       <c r="C5" s="14" t="s">
+        <v>409</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="36">
+        <v>5</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>763</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="36">
+        <v>6</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="36">
+        <v>7</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>766</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="36">
+        <v>8</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>768</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="36">
+        <v>9</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>770</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="36">
+        <v>10</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>772</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="36">
+        <v>11</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="36">
+        <v>12</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="36">
+        <v>13</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>774</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="36">
+        <v>14</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C15" s="14" t="s">
         <v>410</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D15" s="15" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="36">
+        <v>15</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="36">
+        <v>16</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="36">
+        <v>17</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="36">
+        <v>18</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="36">
+        <v>19</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>413</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="36">
+        <v>20</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C21" s="14" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="38">
-        <v>5</v>
-      </c>
-      <c r="B6" s="14" t="s">
+      <c r="D21" s="15" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="36">
+        <v>21</v>
+      </c>
+      <c r="B22" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="C6" s="14" t="s">
-        <v>158</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="38">
-        <v>6</v>
-      </c>
-      <c r="B7" s="14" t="s">
+      <c r="C22" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="36">
+        <v>22</v>
+      </c>
+      <c r="B23" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="C7" s="14" t="s">
-        <v>173</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="38">
-        <v>7</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>174</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="38">
-        <v>8</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>412</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="38">
-        <v>9</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>413</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="38">
-        <v>10</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>175</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="38">
-        <v>11</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>176</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="38">
-        <v>12</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="38">
-        <v>13</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>417</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="38">
-        <v>14</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>415</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="38">
-        <v>15</v>
-      </c>
-      <c r="B16" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>161</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="38">
-        <v>16</v>
-      </c>
-      <c r="B17" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>177</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="38">
-        <v>17</v>
-      </c>
-      <c r="B18" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="C18" s="14" t="s">
+      <c r="C23" s="17" t="s">
         <v>178</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D23" s="18" t="s">
         <v>114</v>
       </c>
     </row>
@@ -6085,10 +9561,10 @@
         <v>118</v>
       </c>
       <c r="C17" s="5" t="s">
+        <v>403</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>404</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -6099,10 +9575,10 @@
         <v>118</v>
       </c>
       <c r="C18" s="5" t="s">
+        <v>405</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>406</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -6113,10 +9589,10 @@
         <v>118</v>
       </c>
       <c r="C19" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>408</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>409</v>
       </c>
     </row>
   </sheetData>

</xml_diff>